<commit_message>
Actualizacion de plan estrategico , estimacion y catalogo de servicios linea base
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Planeacion/Estimación-150204.xlsx
+++ b/qualtcom/Procesos/Planeacion/Estimación-150204.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\via\schoolqtp\qualtcom\Procesos\Planeacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Procesos\Planeacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="129">
   <si>
     <t>Instalaciones</t>
   </si>
@@ -464,6 +464,12 @@
   </si>
   <si>
     <t>Esfuerzo Anual</t>
+  </si>
+  <si>
+    <t>CAMBIOS</t>
+  </si>
+  <si>
+    <t>Estimación VIA</t>
   </si>
 </sst>
 </file>
@@ -574,7 +580,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -590,6 +596,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -747,7 +777,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -844,15 +874,9 @@
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -862,9 +886,6 @@
     <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -886,9 +907,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -907,7 +925,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -927,38 +944,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -969,20 +1032,71 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="4" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -993,93 +1107,96 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1092,62 +1209,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1457,85 +1520,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P26"/>
+  <dimension ref="B1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:F10"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="4" width="14.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="7.140625" style="1" customWidth="1"/>
     <col min="9" max="9" width="28.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="21.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="1" customWidth="1"/>
     <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="46" t="s">
-        <v>71</v>
-      </c>
+    <row r="1" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="95" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="95"/>
     </row>
     <row r="5" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="I5" s="87" t="s">
+      <c r="C5" s="104"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="I5" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="J5" s="87"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="96"/>
     </row>
     <row r="6" spans="2:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="68"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="66" t="s">
+      <c r="B6" s="63"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="49" t="s">
+      <c r="F6" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="G6" s="69" t="s">
+      <c r="G6" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="51" t="s">
+      <c r="I6" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="J6" s="67" t="s">
+      <c r="J6" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="7" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="101" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="89"/>
-      <c r="D7" s="90"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="103"/>
       <c r="E7" s="40">
         <f>Capacidad!J5</f>
-        <v>1680</v>
+        <v>720</v>
       </c>
       <c r="F7" s="40">
         <f>Capacidad!J4</f>
-        <v>1680</v>
-      </c>
-      <c r="G7" s="47">
-        <f>(E7+F7)*$J$14</f>
-        <v>139846</v>
+        <v>1920</v>
+      </c>
+      <c r="G7" s="45">
+        <f>(E7+F7)*$J$15</f>
+        <v>109878.99999999999</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>65</v>
@@ -1548,11 +1615,11 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="88" t="s">
+      <c r="B8" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="89"/>
-      <c r="D8" s="90"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="103"/>
       <c r="E8" s="40">
         <f>Capacidad!R5</f>
         <v>547.20000000000005</v>
@@ -1561,8 +1628,8 @@
         <f>Capacidad!R4</f>
         <v>1094.4000000000001</v>
       </c>
-      <c r="G8" s="47">
-        <f>(E8+F8)*$J$14</f>
+      <c r="G8" s="45">
+        <f>(E8+F8)*$J$15</f>
         <v>68324.759999999995</v>
       </c>
       <c r="I8" s="39" t="s">
@@ -1576,18 +1643,18 @@
       </c>
     </row>
     <row r="9" spans="2:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="88" t="s">
+      <c r="B9" s="101" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="89"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="92">
+      <c r="C9" s="102"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="93">
         <f>Capacidad!D10</f>
         <v>12</v>
       </c>
-      <c r="F9" s="93"/>
-      <c r="G9" s="47">
-        <f>+E9*$K$14</f>
+      <c r="F9" s="94"/>
+      <c r="G9" s="45">
+        <f>+E9*$K$15</f>
         <v>799.45</v>
       </c>
       <c r="I9" s="39" t="s">
@@ -1601,113 +1668,134 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="88" t="s">
+      <c r="B10" s="101" t="s">
         <v>104</v>
       </c>
-      <c r="C10" s="89"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="92">
+      <c r="C10" s="102"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="93">
         <f>Capacidad!D11</f>
         <v>24</v>
       </c>
-      <c r="F10" s="93"/>
-      <c r="G10" s="47">
-        <f>+E10*$J$14</f>
+      <c r="F10" s="94"/>
+      <c r="G10" s="45">
+        <f>+E10*$J$15</f>
         <v>998.89999999999986</v>
       </c>
       <c r="I10" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="85">
+      <c r="J10" s="99">
         <v>389</v>
       </c>
-      <c r="K10" s="85">
+      <c r="K10" s="99">
         <v>389</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="95" t="s">
+      <c r="B11" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="92">
+      <c r="C11" s="98"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="93">
         <f>Capacidad!D12</f>
         <v>6</v>
       </c>
-      <c r="F11" s="93"/>
-      <c r="G11" s="47">
-        <f>+E11*$J$14</f>
+      <c r="F11" s="94"/>
+      <c r="G11" s="45">
+        <f>+E11*$J$15</f>
         <v>249.72499999999997</v>
       </c>
       <c r="I11" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-    </row>
-    <row r="12" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="94" t="s">
+      <c r="J11" s="100"/>
+      <c r="K11" s="100"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="101" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="102"/>
+      <c r="D12" s="103"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="45"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
+    </row>
+    <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="94"/>
-      <c r="D12" s="94"/>
-      <c r="G12" s="42">
-        <f>SUM(G7:G11)</f>
-        <v>210218.83500000002</v>
-      </c>
-      <c r="I12" s="39" t="s">
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="105">
+        <f>SUM(E7:F12)</f>
+        <v>4323.6000000000004</v>
+      </c>
+      <c r="F13" s="106"/>
+      <c r="G13" s="76">
+        <f>SUM(G7:G12)</f>
+        <v>180251.83499999999</v>
+      </c>
+      <c r="I13" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="J12" s="41">
+      <c r="J13" s="41">
         <v>250</v>
       </c>
-      <c r="K12" s="41">
+      <c r="K13" s="41">
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I13" s="43" t="s">
+    <row r="14" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I14" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="J13" s="44">
-        <f>SUM(J7:J12)</f>
+      <c r="J14" s="77">
+        <f>SUM(J7:J13)</f>
         <v>9989</v>
       </c>
-      <c r="K13" s="44">
-        <f>SUM(K7:K12)</f>
+      <c r="K14" s="77">
+        <f>SUM(K7:K13)</f>
         <v>15989</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I14" s="45" t="s">
+    <row r="15" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I15" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="J14" s="44">
-        <f>(J13/30)/8</f>
+      <c r="J15" s="77">
+        <f>(J14/30)/8</f>
         <v>41.62083333333333</v>
       </c>
-      <c r="K14" s="44">
-        <f>(K13/30)/8</f>
+      <c r="K15" s="77">
+        <f>(K14/30)/8</f>
         <v>66.620833333333337</v>
       </c>
     </row>
-    <row r="26" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M26" s="1">
+    <row r="27" spans="13:16" x14ac:dyDescent="0.25">
+      <c r="M27" s="1">
         <f>SUM(Servicios!E23:G23)</f>
         <v>7.7100000000000009</v>
       </c>
-      <c r="P26" s="1">
+      <c r="P27" s="1">
         <f>SUM(Servicios!H23:J23)</f>
         <v>5.2100000000000009</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="17">
     <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="B13:D13"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="K10:K11"/>
-    <mergeCell ref="I5:J5"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
@@ -1717,6 +1805,7 @@
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1746,86 +1835,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="44" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
+      <c r="C4" s="134"/>
+      <c r="D4" s="134"/>
+      <c r="E4" s="134"/>
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
+      <c r="H4" s="134"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="134"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="99"/>
-      <c r="K5" s="99"/>
+      <c r="B5" s="134"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
+      <c r="K5" s="134"/>
     </row>
     <row r="6" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="111" t="s">
+      <c r="C6" s="129" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="96" t="s">
+      <c r="D6" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="102" t="s">
+      <c r="E6" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="103"/>
-      <c r="I6" s="102" t="s">
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="123" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="103"/>
-      <c r="K6" s="96" t="s">
+      <c r="J6" s="125"/>
+      <c r="K6" s="126" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="97"/>
-      <c r="C7" s="112"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="96" t="s">
+      <c r="B7" s="127"/>
+      <c r="C7" s="130"/>
+      <c r="D7" s="127"/>
+      <c r="E7" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="96" t="s">
+      <c r="F7" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="104" t="s">
+      <c r="G7" s="136" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="105"/>
-      <c r="I7" s="104" t="s">
+      <c r="H7" s="137"/>
+      <c r="I7" s="136" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="105"/>
-      <c r="K7" s="97"/>
+      <c r="J7" s="137"/>
+      <c r="K7" s="127"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="98"/>
-      <c r="C8" s="113"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="131"/>
+      <c r="D8" s="128"/>
+      <c r="E8" s="128"/>
+      <c r="F8" s="128"/>
       <c r="G8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1838,16 +1927,16 @@
       <c r="J8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="98"/>
+      <c r="K8" s="128"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="135" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="101">
+      <c r="D9" s="135">
         <v>30</v>
       </c>
       <c r="E9" s="5">
@@ -1868,11 +1957,11 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="101"/>
+      <c r="B10" s="135"/>
       <c r="C10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="101"/>
+      <c r="D10" s="135"/>
       <c r="E10" s="27"/>
       <c r="F10" s="5">
         <v>60</v>
@@ -1891,13 +1980,13 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="135" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="101">
+      <c r="D11" s="135">
         <v>45</v>
       </c>
       <c r="E11" s="5">
@@ -1918,11 +2007,11 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="101"/>
+      <c r="B12" s="135"/>
       <c r="C12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="101"/>
+      <c r="D12" s="135"/>
       <c r="E12" s="28"/>
       <c r="F12" s="5">
         <v>60</v>
@@ -1941,13 +2030,13 @@
       </c>
     </row>
     <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="122" t="s">
         <v>70</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="114">
+      <c r="D13" s="132">
         <v>90</v>
       </c>
       <c r="E13" s="5">
@@ -1968,11 +2057,11 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="109"/>
+      <c r="B14" s="122"/>
       <c r="C14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="100"/>
+      <c r="D14" s="133"/>
       <c r="E14" s="28"/>
       <c r="F14" s="5">
         <v>90</v>
@@ -1993,31 +2082,31 @@
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="121" t="s">
+      <c r="D15" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="121"/>
-      <c r="F15" s="121"/>
-      <c r="G15" s="121"/>
-      <c r="H15" s="121"/>
-      <c r="I15" s="121"/>
-      <c r="J15" s="121"/>
-      <c r="K15" s="121"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
+      <c r="J15" s="113"/>
+      <c r="K15" s="113"/>
     </row>
     <row r="17" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="122" t="s">
+      <c r="B17" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="123"/>
-      <c r="D17" s="123"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="124"/>
-      <c r="I17" s="122" t="s">
+      <c r="C17" s="115"/>
+      <c r="D17" s="115"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="115"/>
+      <c r="G17" s="116"/>
+      <c r="I17" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="123"/>
-      <c r="K17" s="124"/>
+      <c r="J17" s="115"/>
+      <c r="K17" s="116"/>
       <c r="L17" s="3" t="s">
         <v>51</v>
       </c>
@@ -2045,22 +2134,22 @@
       <c r="G18" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="I18" s="106" t="s">
+      <c r="I18" s="117" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="107"/>
-      <c r="K18" s="108"/>
-      <c r="L18" s="125">
+      <c r="J18" s="118"/>
+      <c r="K18" s="119"/>
+      <c r="L18" s="120">
         <v>15</v>
       </c>
-      <c r="M18" s="115">
+      <c r="M18" s="107">
         <f>L18*$E$25</f>
         <v>765</v>
       </c>
       <c r="N18" s="10"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="100" t="s">
+      <c r="B19" s="133" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="12" t="s">
@@ -2078,20 +2167,20 @@
         <v>1500</v>
       </c>
       <c r="G19" s="14">
-        <f>(F19/60)*Estimación!$J$14</f>
+        <f>(F19/60)*Estimación!$J$15</f>
         <v>1040.5208333333333</v>
       </c>
-      <c r="I19" s="106" t="s">
+      <c r="I19" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="J19" s="107"/>
-      <c r="K19" s="108"/>
-      <c r="L19" s="126"/>
-      <c r="M19" s="116"/>
+      <c r="J19" s="118"/>
+      <c r="K19" s="119"/>
+      <c r="L19" s="121"/>
+      <c r="M19" s="108"/>
       <c r="N19" s="10"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="101"/>
+      <c r="B20" s="135"/>
       <c r="C20" s="7" t="s">
         <v>16</v>
       </c>
@@ -2106,14 +2195,14 @@
         <v>210</v>
       </c>
       <c r="G20" s="14">
-        <f>(F20/60)*Estimación!$J$14</f>
+        <f>(F20/60)*Estimación!$J$15</f>
         <v>145.67291666666665</v>
       </c>
-      <c r="I20" s="106" t="s">
+      <c r="I20" s="117" t="s">
         <v>54</v>
       </c>
-      <c r="J20" s="107"/>
-      <c r="K20" s="108"/>
+      <c r="J20" s="118"/>
+      <c r="K20" s="119"/>
       <c r="L20" s="29"/>
       <c r="M20" s="13">
         <f>F25</f>
@@ -2122,7 +2211,7 @@
       <c r="N20" s="10"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="101" t="s">
+      <c r="B21" s="135" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -2140,14 +2229,14 @@
         <v>3450</v>
       </c>
       <c r="G21" s="14">
-        <f>(F21/60)*Estimación!$J$14</f>
+        <f>(F21/60)*Estimación!$J$15</f>
         <v>2393.1979166666665</v>
       </c>
-      <c r="I21" s="106" t="s">
+      <c r="I21" s="117" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="107"/>
-      <c r="K21" s="108"/>
+      <c r="J21" s="118"/>
+      <c r="K21" s="119"/>
       <c r="L21" s="13">
         <v>10</v>
       </c>
@@ -2158,7 +2247,7 @@
       <c r="N21" s="10"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="101"/>
+      <c r="B22" s="135"/>
       <c r="C22" s="7" t="s">
         <v>16</v>
       </c>
@@ -2173,14 +2262,14 @@
         <v>225</v>
       </c>
       <c r="G22" s="14">
-        <f>(F22/60)*Estimación!$J$14</f>
+        <f>(F22/60)*Estimación!$J$15</f>
         <v>156.078125</v>
       </c>
-      <c r="I22" s="117" t="s">
+      <c r="I22" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="J22" s="118"/>
-      <c r="K22" s="119"/>
+      <c r="J22" s="110"/>
+      <c r="K22" s="111"/>
       <c r="L22" s="13">
         <f>SUM(L18:L21)</f>
         <v>25</v>
@@ -2192,7 +2281,7 @@
       <c r="N22" s="10"/>
     </row>
     <row r="23" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="109" t="s">
+      <c r="B23" s="122" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -2210,15 +2299,15 @@
         <v>0</v>
       </c>
       <c r="G23" s="14">
-        <f>(F23/60)*Estimación!$J$14</f>
+        <f>(F23/60)*Estimación!$J$15</f>
         <v>0</v>
       </c>
-      <c r="I23" s="120" t="s">
+      <c r="I23" s="112" t="s">
         <v>56</v>
       </c>
-      <c r="J23" s="120"/>
-      <c r="K23" s="120"/>
-      <c r="L23" s="120"/>
+      <c r="J23" s="112"/>
+      <c r="K23" s="112"/>
+      <c r="L23" s="112"/>
       <c r="M23" s="23">
         <f>M22/60</f>
         <v>122.5</v>
@@ -2228,7 +2317,7 @@
       </c>
     </row>
     <row r="24" spans="2:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="109"/>
+      <c r="B24" s="122"/>
       <c r="C24" s="7" t="s">
         <v>16</v>
       </c>
@@ -2243,17 +2332,17 @@
         <v>1200</v>
       </c>
       <c r="G24" s="14">
-        <f>(F24/60)*Estimación!$J$14</f>
+        <f>(F24/60)*Estimación!$J$15</f>
         <v>832.41666666666663</v>
       </c>
-      <c r="I24" s="120" t="s">
+      <c r="I24" s="112" t="s">
         <v>57</v>
       </c>
-      <c r="J24" s="120"/>
-      <c r="K24" s="120"/>
-      <c r="L24" s="120"/>
+      <c r="J24" s="112"/>
+      <c r="K24" s="112"/>
+      <c r="L24" s="112"/>
       <c r="M24" s="24">
-        <f>M23*Estimación!J14</f>
+        <f>M23*Estimación!J15</f>
         <v>5098.552083333333</v>
       </c>
       <c r="N24" s="10"/>
@@ -2305,22 +2394,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I24:L24"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D13:D14"/>
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="B4:K5"/>
     <mergeCell ref="B19:B20"/>
@@ -2337,6 +2410,22 @@
     <mergeCell ref="I21:K21"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="G7:H7"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I24:L24"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="58" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2687,8 +2776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:G15"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2714,181 +2803,182 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
     </row>
     <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="130"/>
-      <c r="C4" s="128" t="s">
+      <c r="B4" s="161"/>
+      <c r="C4" s="159" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="129"/>
-      <c r="E4" s="129"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
     </row>
     <row r="5" spans="2:10" ht="36.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="131"/>
-      <c r="C5" s="77" t="s">
+      <c r="B5" s="162"/>
+      <c r="C5" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="49" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="132" t="s">
+    <row r="6" spans="2:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="142" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="53">
+      <c r="C6" s="50">
         <v>0.5</v>
       </c>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="G6" s="127" t="s">
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="G6" s="158" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="127"/>
-      <c r="I6" s="127"/>
+      <c r="H6" s="158"/>
+      <c r="I6" s="158"/>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="132"/>
-      <c r="C7" s="78"/>
-      <c r="D7" s="53">
+      <c r="B7" s="142"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="50">
         <v>1</v>
       </c>
-      <c r="E7" s="78"/>
+      <c r="E7" s="71"/>
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
       <c r="I7" s="32"/>
     </row>
     <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="132"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="53">
+      <c r="B8" s="142"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="50">
         <v>2</v>
       </c>
-      <c r="G8" s="127"/>
+      <c r="G8" s="146"/>
       <c r="H8" s="34"/>
-      <c r="I8" s="54"/>
+      <c r="I8" s="51"/>
     </row>
     <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="149" t="s">
+      <c r="B9" s="141" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="53">
+      <c r="C9" s="50">
         <v>1</v>
       </c>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="G9" s="127"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="G9" s="146"/>
       <c r="H9" s="38"/>
-      <c r="I9" s="54"/>
+      <c r="I9" s="51"/>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="132"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="53">
+      <c r="B10" s="142"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="50">
         <v>2</v>
       </c>
-      <c r="E10" s="78"/>
-      <c r="G10" s="127"/>
+      <c r="E10" s="71"/>
+      <c r="G10" s="146"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="54"/>
+      <c r="I10" s="51"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="150"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78"/>
-      <c r="E11" s="53">
+      <c r="B11" s="143"/>
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="50">
         <v>3</v>
       </c>
-      <c r="G11" s="127"/>
+      <c r="G11" s="146"/>
       <c r="H11" s="38"/>
-      <c r="I11" s="54"/>
+      <c r="I11" s="51"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G12" s="127"/>
+      <c r="G12" s="146"/>
       <c r="H12" s="38"/>
-      <c r="I12" s="54"/>
+      <c r="I12" s="51"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G13" s="127"/>
+      <c r="G13" s="146"/>
       <c r="H13" s="34"/>
-      <c r="I13" s="54"/>
+      <c r="I13" s="51"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G14" s="127"/>
+      <c r="G14" s="146"/>
       <c r="H14" s="38"/>
       <c r="I14" s="30"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="141" t="s">
+      <c r="B15" s="150" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="141"/>
-      <c r="D15" s="141"/>
-      <c r="E15" s="143" t="s">
+      <c r="C15" s="150"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="151" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="143"/>
-      <c r="G15" s="143"/>
-      <c r="H15" s="143" t="s">
+      <c r="F15" s="151"/>
+      <c r="G15" s="151"/>
+      <c r="H15" s="151" t="s">
         <v>83</v>
       </c>
-      <c r="I15" s="143"/>
-      <c r="J15" s="143"/>
+      <c r="I15" s="151"/>
+      <c r="J15" s="151"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="141"/>
-      <c r="C16" s="141"/>
-      <c r="D16" s="141"/>
-      <c r="E16" s="49" t="s">
+      <c r="B16" s="150"/>
+      <c r="C16" s="150"/>
+      <c r="D16" s="150"/>
+      <c r="E16" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="F16" s="49" t="s">
+      <c r="F16" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="49" t="s">
+      <c r="G16" s="78" t="s">
         <v>86</v>
       </c>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="78" t="s">
         <v>84</v>
       </c>
-      <c r="I16" s="49" t="s">
+      <c r="I16" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="J16" s="49" t="s">
+      <c r="J16" s="78" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="142" t="s">
+      <c r="B17" s="145" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="142"/>
-      <c r="D17" s="142"/>
-      <c r="E17" s="134">
+      <c r="C17" s="145"/>
+      <c r="D17" s="145"/>
+      <c r="E17" s="144">
         <v>0.16</v>
       </c>
-      <c r="F17" s="134">
+      <c r="F17" s="144">
         <v>0.16</v>
       </c>
-      <c r="G17" s="134">
+      <c r="G17" s="144">
         <v>0.16</v>
       </c>
-      <c r="H17" s="134">
+      <c r="H17" s="144">
         <v>0.16</v>
       </c>
-      <c r="I17" s="134">
+      <c r="I17" s="144">
         <v>0.16</v>
       </c>
-      <c r="J17" s="134">
+      <c r="J17" s="144">
         <v>0.16</v>
       </c>
       <c r="K17" s="30"/>
@@ -2901,17 +2991,17 @@
       <c r="R17" s="30"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="142" t="s">
+      <c r="B18" s="145" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="142"/>
-      <c r="D18" s="142"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
-      <c r="G18" s="134"/>
-      <c r="H18" s="134"/>
-      <c r="I18" s="134"/>
-      <c r="J18" s="134"/>
+      <c r="C18" s="145"/>
+      <c r="D18" s="145"/>
+      <c r="E18" s="144"/>
+      <c r="F18" s="144"/>
+      <c r="G18" s="144"/>
+      <c r="H18" s="144"/>
+      <c r="I18" s="144"/>
+      <c r="J18" s="144"/>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
       <c r="M18" s="30"/>
@@ -2922,274 +3012,274 @@
       <c r="R18" s="30"/>
     </row>
     <row r="19" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="142" t="s">
+      <c r="B19" s="145" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="142"/>
-      <c r="D19" s="142"/>
-      <c r="E19" s="134">
+      <c r="C19" s="145"/>
+      <c r="D19" s="145"/>
+      <c r="E19" s="144">
         <v>0.25</v>
       </c>
-      <c r="F19" s="134">
+      <c r="F19" s="144">
         <v>0.25</v>
       </c>
-      <c r="G19" s="134">
+      <c r="G19" s="144">
         <v>0.25</v>
       </c>
-      <c r="H19" s="134">
+      <c r="H19" s="144">
         <v>0.25</v>
       </c>
-      <c r="I19" s="134">
+      <c r="I19" s="144">
         <v>0.25</v>
       </c>
-      <c r="J19" s="134">
+      <c r="J19" s="144">
         <v>0.25</v>
       </c>
-      <c r="K19" s="147"/>
-      <c r="L19" s="147"/>
-      <c r="M19" s="147"/>
-      <c r="N19" s="64"/>
-      <c r="O19" s="64"/>
-      <c r="P19" s="64"/>
-      <c r="Q19" s="144"/>
+      <c r="K19" s="149"/>
+      <c r="L19" s="149"/>
+      <c r="M19" s="149"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="60"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="147"/>
       <c r="R19" s="30"/>
     </row>
     <row r="20" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="142" t="s">
+      <c r="B20" s="145" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="142"/>
-      <c r="D20" s="142"/>
-      <c r="E20" s="134"/>
-      <c r="F20" s="134"/>
-      <c r="G20" s="134"/>
-      <c r="H20" s="134"/>
-      <c r="I20" s="134"/>
-      <c r="J20" s="134"/>
-      <c r="K20" s="147"/>
-      <c r="L20" s="147"/>
-      <c r="M20" s="147"/>
-      <c r="N20" s="64"/>
-      <c r="O20" s="64"/>
-      <c r="P20" s="64"/>
-      <c r="Q20" s="144"/>
+      <c r="C20" s="145"/>
+      <c r="D20" s="145"/>
+      <c r="E20" s="144"/>
+      <c r="F20" s="144"/>
+      <c r="G20" s="144"/>
+      <c r="H20" s="144"/>
+      <c r="I20" s="144"/>
+      <c r="J20" s="144"/>
+      <c r="K20" s="149"/>
+      <c r="L20" s="149"/>
+      <c r="M20" s="149"/>
+      <c r="N20" s="60"/>
+      <c r="O20" s="60"/>
+      <c r="P20" s="60"/>
+      <c r="Q20" s="147"/>
       <c r="R20" s="30"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="138" t="s">
+      <c r="B21" s="155" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="139"/>
-      <c r="D21" s="140"/>
-      <c r="E21" s="50">
+      <c r="C21" s="156"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="47">
         <v>0.16</v>
       </c>
-      <c r="F21" s="50">
+      <c r="F21" s="47">
         <v>0.16</v>
       </c>
-      <c r="G21" s="50">
+      <c r="G21" s="47">
         <v>0.16</v>
       </c>
-      <c r="H21" s="50">
+      <c r="H21" s="47">
         <v>0.16</v>
       </c>
-      <c r="I21" s="50">
+      <c r="I21" s="47">
         <v>0.16</v>
       </c>
-      <c r="J21" s="50">
+      <c r="J21" s="47">
         <v>0.16</v>
       </c>
-      <c r="K21" s="145"/>
-      <c r="L21" s="145"/>
-      <c r="M21" s="145"/>
-      <c r="N21" s="59"/>
-      <c r="O21" s="59"/>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="146"/>
-      <c r="R21" s="58"/>
+      <c r="K21" s="140"/>
+      <c r="L21" s="140"/>
+      <c r="M21" s="140"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="55"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="148"/>
+      <c r="R21" s="54"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="142" t="s">
+      <c r="B22" s="145" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="142"/>
-      <c r="D22" s="142"/>
-      <c r="E22" s="57">
+      <c r="C22" s="145"/>
+      <c r="D22" s="145"/>
+      <c r="E22" s="79">
         <f>Servicios!C9</f>
         <v>1</v>
       </c>
-      <c r="F22" s="57">
+      <c r="F22" s="79">
         <f>Servicios!D10</f>
         <v>2</v>
       </c>
-      <c r="G22" s="57">
+      <c r="G22" s="79">
         <f>Servicios!E11</f>
         <v>3</v>
       </c>
-      <c r="H22" s="75">
+      <c r="H22" s="80">
         <f>Servicios!C6</f>
         <v>0.5</v>
       </c>
-      <c r="I22" s="76">
+      <c r="I22" s="81">
         <f>Servicios!D7</f>
         <v>1</v>
       </c>
-      <c r="J22" s="76">
+      <c r="J22" s="81">
         <f>Servicios!E8</f>
         <v>2</v>
       </c>
-      <c r="K22" s="145"/>
-      <c r="L22" s="145"/>
-      <c r="M22" s="145"/>
-      <c r="N22" s="59"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="59"/>
-      <c r="Q22" s="146"/>
-      <c r="R22" s="58"/>
+      <c r="K22" s="140"/>
+      <c r="L22" s="140"/>
+      <c r="M22" s="140"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="148"/>
+      <c r="R22" s="54"/>
     </row>
     <row r="23" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="135" t="s">
+      <c r="B23" s="152" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="136"/>
-      <c r="D23" s="137"/>
-      <c r="E23" s="48">
+      <c r="C23" s="153"/>
+      <c r="D23" s="154"/>
+      <c r="E23" s="82">
         <f t="shared" ref="E23:J23" si="0">SUM(E17:E22)</f>
         <v>1.57</v>
       </c>
-      <c r="F23" s="48">
+      <c r="F23" s="82">
         <f t="shared" si="0"/>
         <v>2.5700000000000003</v>
       </c>
-      <c r="G23" s="48">
+      <c r="G23" s="82">
         <f t="shared" si="0"/>
         <v>3.5700000000000003</v>
       </c>
-      <c r="H23" s="48">
+      <c r="H23" s="82">
         <f t="shared" si="0"/>
         <v>1.07</v>
       </c>
-      <c r="I23" s="48">
+      <c r="I23" s="82">
         <f t="shared" si="0"/>
         <v>1.57</v>
       </c>
-      <c r="J23" s="48">
+      <c r="J23" s="82">
         <f t="shared" si="0"/>
         <v>2.5700000000000003</v>
       </c>
-      <c r="K23" s="145"/>
-      <c r="L23" s="145"/>
-      <c r="M23" s="145"/>
-      <c r="N23" s="59"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59"/>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="58"/>
+      <c r="K23" s="140"/>
+      <c r="L23" s="140"/>
+      <c r="M23" s="140"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="54"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F24" s="30"/>
-      <c r="G24" s="70"/>
+      <c r="G24" s="65"/>
       <c r="H24" s="38"/>
-      <c r="I24" s="54"/>
+      <c r="I24" s="51"/>
       <c r="J24" s="32"/>
-      <c r="K24" s="145"/>
-      <c r="L24" s="145"/>
-      <c r="M24" s="145"/>
-      <c r="N24" s="59"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="58"/>
+      <c r="K24" s="140"/>
+      <c r="L24" s="140"/>
+      <c r="M24" s="140"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="55"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="51"/>
+      <c r="R24" s="54"/>
     </row>
     <row r="25" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F25" s="30"/>
-      <c r="G25" s="127"/>
+      <c r="G25" s="146"/>
       <c r="H25" s="34"/>
-      <c r="I25" s="54"/>
+      <c r="I25" s="51"/>
       <c r="J25" s="33"/>
-      <c r="K25" s="145"/>
-      <c r="L25" s="145"/>
-      <c r="M25" s="145"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="146"/>
-      <c r="R25" s="58"/>
+      <c r="K25" s="140"/>
+      <c r="L25" s="140"/>
+      <c r="M25" s="140"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="148"/>
+      <c r="R25" s="54"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F26" s="30"/>
-      <c r="G26" s="127"/>
+      <c r="G26" s="146"/>
       <c r="H26" s="38"/>
-      <c r="I26" s="54"/>
+      <c r="I26" s="51"/>
       <c r="J26" s="33"/>
-      <c r="K26" s="145"/>
-      <c r="L26" s="145"/>
-      <c r="M26" s="145"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="146"/>
-      <c r="R26" s="58"/>
+      <c r="K26" s="140"/>
+      <c r="L26" s="140"/>
+      <c r="M26" s="140"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="148"/>
+      <c r="R26" s="54"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F27" s="30"/>
-      <c r="G27" s="127"/>
+      <c r="G27" s="146"/>
       <c r="H27" s="34"/>
-      <c r="I27" s="54"/>
+      <c r="I27" s="51"/>
       <c r="J27" s="33"/>
-      <c r="K27" s="145"/>
-      <c r="L27" s="145"/>
-      <c r="M27" s="145"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="146"/>
-      <c r="R27" s="58"/>
+      <c r="K27" s="140"/>
+      <c r="L27" s="140"/>
+      <c r="M27" s="140"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="55"/>
+      <c r="P27" s="55"/>
+      <c r="Q27" s="148"/>
+      <c r="R27" s="54"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F28" s="30"/>
-      <c r="G28" s="127"/>
+      <c r="G28" s="146"/>
       <c r="H28" s="38"/>
-      <c r="I28" s="54"/>
+      <c r="I28" s="51"/>
       <c r="J28" s="33"/>
-      <c r="K28" s="145"/>
-      <c r="L28" s="145"/>
-      <c r="M28" s="145"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="55"/>
-      <c r="R28" s="58"/>
+      <c r="K28" s="140"/>
+      <c r="L28" s="140"/>
+      <c r="M28" s="140"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="55"/>
+      <c r="Q28" s="52"/>
+      <c r="R28" s="54"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F29" s="30"/>
-      <c r="G29" s="133"/>
-      <c r="H29" s="133"/>
-      <c r="I29" s="54"/>
+      <c r="G29" s="138"/>
+      <c r="H29" s="138"/>
+      <c r="I29" s="51"/>
       <c r="J29" s="33"/>
-      <c r="K29" s="145"/>
-      <c r="L29" s="145"/>
-      <c r="M29" s="145"/>
-      <c r="N29" s="59"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="54"/>
-      <c r="R29" s="58"/>
+      <c r="K29" s="140"/>
+      <c r="L29" s="140"/>
+      <c r="M29" s="140"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="55"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="54"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F30" s="30"/>
-      <c r="G30" s="133"/>
-      <c r="H30" s="133"/>
-      <c r="I30" s="56"/>
+      <c r="G30" s="138"/>
+      <c r="H30" s="138"/>
+      <c r="I30" s="53"/>
       <c r="J30" s="33"/>
-      <c r="K30" s="133"/>
-      <c r="L30" s="133"/>
-      <c r="M30" s="133"/>
-      <c r="N30" s="60"/>
-      <c r="O30" s="60"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="55"/>
-      <c r="R30" s="58"/>
+      <c r="K30" s="138"/>
+      <c r="L30" s="138"/>
+      <c r="M30" s="138"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="56"/>
+      <c r="P30" s="56"/>
+      <c r="Q30" s="52"/>
+      <c r="R30" s="54"/>
     </row>
     <row r="31" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="F31" s="30"/>
@@ -3197,14 +3287,14 @@
       <c r="H31" s="31"/>
       <c r="I31" s="34"/>
       <c r="J31" s="33"/>
-      <c r="K31" s="148"/>
-      <c r="L31" s="148"/>
-      <c r="M31" s="148"/>
-      <c r="N31" s="148"/>
-      <c r="O31" s="148"/>
-      <c r="P31" s="148"/>
-      <c r="Q31" s="61"/>
-      <c r="R31" s="62"/>
+      <c r="K31" s="139"/>
+      <c r="L31" s="139"/>
+      <c r="M31" s="139"/>
+      <c r="N31" s="139"/>
+      <c r="O31" s="139"/>
+      <c r="P31" s="139"/>
+      <c r="Q31" s="57"/>
+      <c r="R31" s="58"/>
     </row>
     <row r="32" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="F32" s="30"/>
@@ -3212,13 +3302,13 @@
       <c r="H32" s="31"/>
       <c r="I32" s="38"/>
       <c r="J32" s="33"/>
-      <c r="K32" s="148"/>
-      <c r="L32" s="148"/>
-      <c r="M32" s="148"/>
-      <c r="N32" s="148"/>
-      <c r="O32" s="148"/>
-      <c r="P32" s="148"/>
-      <c r="Q32" s="63"/>
+      <c r="K32" s="139"/>
+      <c r="L32" s="139"/>
+      <c r="M32" s="139"/>
+      <c r="N32" s="139"/>
+      <c r="O32" s="139"/>
+      <c r="P32" s="139"/>
+      <c r="Q32" s="59"/>
       <c r="R32" s="30"/>
     </row>
     <row r="33" spans="6:18" x14ac:dyDescent="0.25">
@@ -3234,7 +3324,7 @@
       <c r="O33" s="30"/>
       <c r="P33" s="30"/>
       <c r="Q33" s="35"/>
-      <c r="R33" s="58"/>
+      <c r="R33" s="54"/>
     </row>
     <row r="34" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F34" s="30"/>
@@ -3252,7 +3342,39 @@
       <c r="J35" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="48">
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="G29:H30"/>
+    <mergeCell ref="G25:G28"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="B15:D16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="Q25:Q27"/>
+    <mergeCell ref="K19:M20"/>
+    <mergeCell ref="Q21:Q22"/>
     <mergeCell ref="K30:M30"/>
     <mergeCell ref="K31:P31"/>
     <mergeCell ref="K32:P32"/>
@@ -3269,37 +3391,6 @@
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="G8:G11"/>
     <mergeCell ref="J17:J18"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="Q25:Q27"/>
-    <mergeCell ref="K19:M20"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="B15:D16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="G29:H30"/>
-    <mergeCell ref="G25:G28"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="I19:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3311,233 +3402,231 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" style="71" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="66" customWidth="1"/>
     <col min="11" max="12" width="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5" style="71" customWidth="1"/>
-    <col min="15" max="15" width="5" style="71" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" style="66" customWidth="1"/>
+    <col min="15" max="15" width="5" style="66" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="74"/>
-      <c r="B2" s="151" t="s">
+      <c r="A2" s="69"/>
+      <c r="B2" s="163" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151" t="s">
+      <c r="C2" s="163"/>
+      <c r="D2" s="163" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="151"/>
-      <c r="F2" s="151" t="s">
+      <c r="E2" s="163"/>
+      <c r="F2" s="163" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="151"/>
-      <c r="H2" s="79" t="s">
+      <c r="G2" s="163"/>
+      <c r="H2" s="84" t="s">
         <v>98</v>
       </c>
-      <c r="I2" s="79" t="s">
+      <c r="I2" s="84" t="s">
         <v>99</v>
       </c>
-      <c r="J2" s="79" t="s">
+      <c r="J2" s="84" t="s">
         <v>121</v>
       </c>
-      <c r="K2" s="109" t="s">
+      <c r="K2" s="158" t="s">
         <v>101</v>
       </c>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="109"/>
-      <c r="O2" s="109"/>
-      <c r="P2" s="109"/>
-      <c r="Q2" s="79" t="s">
+      <c r="L2" s="158"/>
+      <c r="M2" s="158"/>
+      <c r="N2" s="158"/>
+      <c r="O2" s="158"/>
+      <c r="P2" s="158"/>
+      <c r="Q2" s="84" t="s">
         <v>102</v>
       </c>
-      <c r="R2" s="79" t="s">
+      <c r="R2" s="84" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="74"/>
-      <c r="B3" s="72" t="s">
+      <c r="A3" s="69"/>
+      <c r="B3" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="72" t="s">
+      <c r="F3" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="G3" s="72" t="s">
+      <c r="G3" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="151" t="s">
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="164" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="151"/>
-      <c r="M3" s="151" t="s">
+      <c r="L3" s="164"/>
+      <c r="M3" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="N3" s="151"/>
-      <c r="O3" s="151" t="s">
+      <c r="N3" s="164"/>
+      <c r="O3" s="164" t="s">
         <v>86</v>
       </c>
-      <c r="P3" s="151"/>
-      <c r="Q3" s="72"/>
-      <c r="R3" s="80"/>
+      <c r="P3" s="164"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="72"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="72">
-        <v>4</v>
-      </c>
-      <c r="C4" s="72">
+      <c r="B4" s="67">
+        <v>6</v>
+      </c>
+      <c r="C4" s="67">
         <v>0.5</v>
       </c>
-      <c r="D4" s="72">
-        <v>3</v>
-      </c>
-      <c r="E4" s="72">
+      <c r="D4" s="67">
         <v>1</v>
       </c>
-      <c r="F4" s="72">
+      <c r="E4" s="67">
         <v>1</v>
       </c>
-      <c r="G4" s="72">
+      <c r="F4" s="67">
+        <v>1</v>
+      </c>
+      <c r="G4" s="67">
         <v>2</v>
       </c>
-      <c r="H4" s="72">
-        <f>(B4*C4)+(D4*E4)+(F4*G4)</f>
-        <v>7</v>
-      </c>
-      <c r="I4" s="72">
+      <c r="H4" s="67">
+        <v>8</v>
+      </c>
+      <c r="I4" s="67">
         <f>H4*20</f>
-        <v>140</v>
-      </c>
-      <c r="J4" s="80">
+        <v>160</v>
+      </c>
+      <c r="J4" s="72">
         <f>I4*12</f>
-        <v>1680</v>
-      </c>
-      <c r="K4" s="72">
+        <v>1920</v>
+      </c>
+      <c r="K4" s="67">
         <f>SUM(Servicios!H17:H21)</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="L4" s="72">
+      <c r="L4" s="67">
         <f>(K4*B4)*20</f>
-        <v>45.600000000000009</v>
-      </c>
-      <c r="M4" s="72">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="M4" s="67">
         <f>SUM(Servicios!I17:I21)</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="N4" s="72">
+      <c r="N4" s="67">
         <f>(M4*D4)*20</f>
-        <v>34.200000000000003</v>
-      </c>
-      <c r="O4" s="72">
+        <v>11.400000000000002</v>
+      </c>
+      <c r="O4" s="67">
         <f>SUM(Servicios!J17:J21)</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="P4" s="72">
+      <c r="P4" s="67">
         <f>(O4*F4)*20</f>
         <v>11.400000000000002</v>
       </c>
-      <c r="Q4" s="72">
+      <c r="Q4" s="67">
         <f>SUM(L4,N4,P4)</f>
         <v>91.200000000000017</v>
       </c>
-      <c r="R4" s="80">
+      <c r="R4" s="72">
         <f>Q4*12</f>
         <v>1094.4000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="85" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="72">
+      <c r="B5" s="67">
         <v>2</v>
       </c>
-      <c r="C5" s="72">
+      <c r="C5" s="67">
         <v>1</v>
       </c>
-      <c r="D5" s="72">
+      <c r="D5" s="67">
         <v>1</v>
       </c>
-      <c r="E5" s="72">
+      <c r="E5" s="67">
         <v>2</v>
       </c>
-      <c r="F5" s="72">
+      <c r="F5" s="67">
         <v>1</v>
       </c>
-      <c r="G5" s="72">
+      <c r="G5" s="67">
         <v>3</v>
       </c>
-      <c r="H5" s="72">
-        <f>(B5*C5)+(D5*E5)+(F5*G5)</f>
-        <v>7</v>
-      </c>
-      <c r="I5" s="72">
+      <c r="H5" s="67">
+        <v>3</v>
+      </c>
+      <c r="I5" s="67">
         <f>H5*20</f>
-        <v>140</v>
-      </c>
-      <c r="J5" s="80">
+        <v>60</v>
+      </c>
+      <c r="J5" s="72">
         <f>I5*12</f>
-        <v>1680</v>
-      </c>
-      <c r="K5" s="72">
+        <v>720</v>
+      </c>
+      <c r="K5" s="67">
         <f>SUM(Servicios!E17:E21)</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="L5" s="72">
+      <c r="L5" s="67">
         <f>(K5*B5)*20</f>
         <v>22.800000000000004</v>
       </c>
-      <c r="M5" s="72">
+      <c r="M5" s="67">
         <f>SUM(Servicios!F17:F21)</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="N5" s="72">
+      <c r="N5" s="67">
         <f>(M5*D5)*20</f>
         <v>11.400000000000002</v>
       </c>
-      <c r="O5" s="72">
+      <c r="O5" s="67">
         <f>SUM(Servicios!G17:G21)</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="P5" s="72">
+      <c r="P5" s="67">
         <f>(O5*F5)*20</f>
         <v>11.400000000000002</v>
       </c>
-      <c r="Q5" s="72">
+      <c r="Q5" s="67">
         <f>SUM(L5,N5,P5)</f>
         <v>45.600000000000009</v>
       </c>
-      <c r="R5" s="80">
+      <c r="R5" s="72">
         <f>Q5*12</f>
         <v>547.20000000000005</v>
       </c>
@@ -3548,50 +3637,50 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="80"/>
-      <c r="B9" s="79" t="s">
+      <c r="A9" s="83"/>
+      <c r="B9" s="84" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="79" t="s">
+      <c r="C9" s="83"/>
+      <c r="D9" s="84" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="86" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="80">
+      <c r="B10" s="72">
         <v>1</v>
       </c>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80">
+      <c r="C10" s="72"/>
+      <c r="D10" s="72">
         <f>B10*12</f>
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="80" t="s">
+      <c r="A11" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="80">
+      <c r="B11" s="72">
         <v>2</v>
       </c>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80">
+      <c r="C11" s="72"/>
+      <c r="D11" s="72">
         <f>B11*12</f>
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="85" t="s">
         <v>123</v>
       </c>
-      <c r="B12" s="80">
+      <c r="B12" s="72">
         <v>0.5</v>
       </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="84">
+      <c r="C12" s="72"/>
+      <c r="D12" s="74">
         <f>B12*12</f>
         <v>6</v>
       </c>
@@ -3616,106 +3705,106 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="71" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
+    <row r="1" spans="1:3" s="66" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="89" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="87" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="90" t="s">
         <v>109</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="90" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="90" t="s">
         <v>110</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="92" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="90" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="66"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="87" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="87" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="90" t="s">
         <v>113</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="90" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="71" t="s">
+      <c r="C9" s="90" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="90" t="s">
         <v>114</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="90" t="s">
         <v>116</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="90" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="90" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="83"/>
+      <c r="A12" s="73"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="83"/>
+      <c r="A13" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizacion de plan de estimacion tras defecto encontrado en auditoria(no se definia si los costos eran anuales o mensuales)
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Planeacion/Estimación-150204.xlsx
+++ b/qualtcom/Procesos/Planeacion/Estimación-150204.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Procesos\Planeacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\qtp\qualtcom\Procesos\Planeacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="131">
   <si>
     <t>Instalaciones</t>
   </si>
@@ -373,9 +373,6 @@
     <t>*La capacidad es contemplando dos recursos de medio tiempo</t>
   </si>
   <si>
-    <t>Esfuerzo Mantenimiento preventivo</t>
-  </si>
-  <si>
     <t>Correctivo</t>
   </si>
   <si>
@@ -470,6 +467,15 @@
   </si>
   <si>
     <t>Estimación VIA</t>
+  </si>
+  <si>
+    <t>Esfuerzo Mantenimiento preventivo Anual</t>
+  </si>
+  <si>
+    <t>Esfuerzo por mantenimiento correctivo Anual</t>
+  </si>
+  <si>
+    <t>Costo Anual</t>
   </si>
 </sst>
 </file>
@@ -999,6 +1005,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1023,15 +1038,6 @@
     <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1041,6 +1047,63 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1071,143 +1134,86 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1522,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,7 +1538,7 @@
     <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="2.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="7.140625" style="1" customWidth="1"/>
@@ -1543,10 +1549,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="95" t="s">
-        <v>128</v>
-      </c>
-      <c r="C1" s="95"/>
+      <c r="B1" s="98" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="98"/>
     </row>
     <row r="5" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="104" t="s">
@@ -1554,27 +1560,27 @@
       </c>
       <c r="C5" s="104"/>
       <c r="D5" s="104"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="I5" s="96" t="s">
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="I5" s="99" t="s">
         <v>61</v>
       </c>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-    </row>
-    <row r="6" spans="2:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="99"/>
+      <c r="K5" s="99"/>
+    </row>
+    <row r="6" spans="2:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="63"/>
       <c r="C6" s="68"/>
       <c r="D6" s="64"/>
       <c r="E6" s="61" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="F6" s="46" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="G6" s="64" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="I6" s="48" t="s">
         <v>62</v>
@@ -1583,15 +1589,15 @@
         <v>63</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="101" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="102"/>
-      <c r="D7" s="103"/>
+      <c r="B7" s="93" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="94"/>
+      <c r="D7" s="95"/>
       <c r="E7" s="40">
         <f>Capacidad!J5</f>
         <v>720</v>
@@ -1615,11 +1621,11 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="103"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="95"/>
       <c r="E8" s="40">
         <f>Capacidad!R5</f>
         <v>547.20000000000005</v>
@@ -1643,16 +1649,16 @@
       </c>
     </row>
     <row r="9" spans="2:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="101" t="s">
-        <v>105</v>
-      </c>
-      <c r="C9" s="102"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="93">
+      <c r="B9" s="93" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="94"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="96">
         <f>Capacidad!D10</f>
         <v>12</v>
       </c>
-      <c r="F9" s="94"/>
+      <c r="F9" s="97"/>
       <c r="G9" s="45">
         <f>+E9*$K$15</f>
         <v>799.45</v>
@@ -1668,16 +1674,16 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="101" t="s">
-        <v>104</v>
-      </c>
-      <c r="C10" s="102"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="93">
+      <c r="B10" s="93" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="94"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="96">
         <f>Capacidad!D11</f>
         <v>24</v>
       </c>
-      <c r="F10" s="94"/>
+      <c r="F10" s="97"/>
       <c r="G10" s="45">
         <f>+E10*$J$15</f>
         <v>998.89999999999986</v>
@@ -1685,24 +1691,24 @@
       <c r="I10" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="99">
+      <c r="J10" s="102">
         <v>389</v>
       </c>
-      <c r="K10" s="99">
+      <c r="K10" s="102">
         <v>389</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="93">
+      <c r="C11" s="101"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="96">
         <f>Capacidad!D12</f>
         <v>6</v>
       </c>
-      <c r="F11" s="94"/>
+      <c r="F11" s="97"/>
       <c r="G11" s="45">
         <f>+E11*$J$15</f>
         <v>249.72499999999997</v>
@@ -1710,28 +1716,28 @@
       <c r="I11" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="J11" s="100"/>
-      <c r="K11" s="100"/>
+      <c r="J11" s="103"/>
+      <c r="K11" s="103"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="101" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="102"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="94"/>
+      <c r="B12" s="93" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="94"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="96"/>
+      <c r="F12" s="97"/>
       <c r="G12" s="45"/>
       <c r="I12" s="39"/>
       <c r="J12" s="75"/>
       <c r="K12" s="75"/>
     </row>
     <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="97" t="s">
+      <c r="B13" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
       <c r="E13" s="105">
         <f>SUM(E7:F12)</f>
         <v>4323.6000000000004</v>
@@ -1789,6 +1795,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="B1:C1"/>
@@ -1805,7 +1812,6 @@
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1840,81 +1846,81 @@
       </c>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="134" t="s">
+      <c r="B4" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="134"/>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
-      <c r="F4" s="134"/>
-      <c r="G4" s="134"/>
-      <c r="H4" s="134"/>
-      <c r="I4" s="134"/>
-      <c r="J4" s="134"/>
-      <c r="K4" s="134"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="110"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
+      <c r="K4" s="110"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="134"/>
-      <c r="C5" s="134"/>
-      <c r="D5" s="134"/>
-      <c r="E5" s="134"/>
-      <c r="F5" s="134"/>
-      <c r="G5" s="134"/>
-      <c r="H5" s="134"/>
-      <c r="I5" s="134"/>
-      <c r="J5" s="134"/>
-      <c r="K5" s="134"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="110"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="110"/>
+      <c r="I5" s="110"/>
+      <c r="J5" s="110"/>
+      <c r="K5" s="110"/>
     </row>
     <row r="6" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="129" t="s">
+      <c r="C6" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="126" t="s">
+      <c r="D6" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="123" t="s">
+      <c r="E6" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="124"/>
-      <c r="G6" s="124"/>
-      <c r="H6" s="125"/>
-      <c r="I6" s="123" t="s">
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="114"/>
+      <c r="I6" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="125"/>
-      <c r="K6" s="126" t="s">
+      <c r="J6" s="114"/>
+      <c r="K6" s="107" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="127"/>
-      <c r="C7" s="130"/>
-      <c r="D7" s="127"/>
-      <c r="E7" s="126" t="s">
+      <c r="B7" s="108"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="108"/>
+      <c r="E7" s="107" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="126" t="s">
+      <c r="F7" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="136" t="s">
+      <c r="G7" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="137"/>
-      <c r="I7" s="136" t="s">
+      <c r="H7" s="116"/>
+      <c r="I7" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="137"/>
-      <c r="K7" s="127"/>
+      <c r="J7" s="116"/>
+      <c r="K7" s="108"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="128"/>
-      <c r="C8" s="131"/>
-      <c r="D8" s="128"/>
-      <c r="E8" s="128"/>
-      <c r="F8" s="128"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="124"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
       <c r="G8" s="3" t="s">
         <v>12</v>
       </c>
@@ -1927,16 +1933,16 @@
       <c r="J8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="128"/>
+      <c r="K8" s="109"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="135" t="s">
+      <c r="B9" s="112" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="135">
+      <c r="D9" s="112">
         <v>30</v>
       </c>
       <c r="E9" s="5">
@@ -1957,11 +1963,11 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="135"/>
+      <c r="B10" s="112"/>
       <c r="C10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="135"/>
+      <c r="D10" s="112"/>
       <c r="E10" s="27"/>
       <c r="F10" s="5">
         <v>60</v>
@@ -1980,13 +1986,13 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="135" t="s">
+      <c r="B11" s="112" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="135">
+      <c r="D11" s="112">
         <v>45</v>
       </c>
       <c r="E11" s="5">
@@ -2007,11 +2013,11 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="135"/>
+      <c r="B12" s="112"/>
       <c r="C12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="135"/>
+      <c r="D12" s="112"/>
       <c r="E12" s="28"/>
       <c r="F12" s="5">
         <v>60</v>
@@ -2030,13 +2036,13 @@
       </c>
     </row>
     <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="122" t="s">
+      <c r="B13" s="120" t="s">
         <v>70</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="132">
+      <c r="D13" s="125">
         <v>90</v>
       </c>
       <c r="E13" s="5">
@@ -2057,11 +2063,11 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="122"/>
+      <c r="B14" s="120"/>
       <c r="C14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="133"/>
+      <c r="D14" s="111"/>
       <c r="E14" s="28"/>
       <c r="F14" s="5">
         <v>90</v>
@@ -2082,31 +2088,31 @@
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="113" t="s">
+      <c r="D15" s="132" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="113"/>
-      <c r="F15" s="113"/>
-      <c r="G15" s="113"/>
-      <c r="H15" s="113"/>
-      <c r="I15" s="113"/>
-      <c r="J15" s="113"/>
-      <c r="K15" s="113"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="132"/>
+      <c r="G15" s="132"/>
+      <c r="H15" s="132"/>
+      <c r="I15" s="132"/>
+      <c r="J15" s="132"/>
+      <c r="K15" s="132"/>
     </row>
     <row r="17" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="114" t="s">
+      <c r="B17" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="115"/>
-      <c r="D17" s="115"/>
-      <c r="E17" s="115"/>
-      <c r="F17" s="115"/>
-      <c r="G17" s="116"/>
-      <c r="I17" s="114" t="s">
+      <c r="C17" s="134"/>
+      <c r="D17" s="134"/>
+      <c r="E17" s="134"/>
+      <c r="F17" s="134"/>
+      <c r="G17" s="135"/>
+      <c r="I17" s="133" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="115"/>
-      <c r="K17" s="116"/>
+      <c r="J17" s="134"/>
+      <c r="K17" s="135"/>
       <c r="L17" s="3" t="s">
         <v>51</v>
       </c>
@@ -2139,17 +2145,17 @@
       </c>
       <c r="J18" s="118"/>
       <c r="K18" s="119"/>
-      <c r="L18" s="120">
+      <c r="L18" s="136">
         <v>15</v>
       </c>
-      <c r="M18" s="107">
+      <c r="M18" s="126">
         <f>L18*$E$25</f>
         <v>765</v>
       </c>
       <c r="N18" s="10"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="133" t="s">
+      <c r="B19" s="111" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="12" t="s">
@@ -2175,12 +2181,12 @@
       </c>
       <c r="J19" s="118"/>
       <c r="K19" s="119"/>
-      <c r="L19" s="121"/>
-      <c r="M19" s="108"/>
+      <c r="L19" s="137"/>
+      <c r="M19" s="127"/>
       <c r="N19" s="10"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="135"/>
+      <c r="B20" s="112"/>
       <c r="C20" s="7" t="s">
         <v>16</v>
       </c>
@@ -2211,7 +2217,7 @@
       <c r="N20" s="10"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="135" t="s">
+      <c r="B21" s="112" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -2247,7 +2253,7 @@
       <c r="N21" s="10"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="135"/>
+      <c r="B22" s="112"/>
       <c r="C22" s="7" t="s">
         <v>16</v>
       </c>
@@ -2265,11 +2271,11 @@
         <f>(F22/60)*Estimación!$J$15</f>
         <v>156.078125</v>
       </c>
-      <c r="I22" s="109" t="s">
+      <c r="I22" s="128" t="s">
         <v>40</v>
       </c>
-      <c r="J22" s="110"/>
-      <c r="K22" s="111"/>
+      <c r="J22" s="129"/>
+      <c r="K22" s="130"/>
       <c r="L22" s="13">
         <f>SUM(L18:L21)</f>
         <v>25</v>
@@ -2281,7 +2287,7 @@
       <c r="N22" s="10"/>
     </row>
     <row r="23" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="122" t="s">
+      <c r="B23" s="120" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="4" t="s">
@@ -2302,12 +2308,12 @@
         <f>(F23/60)*Estimación!$J$15</f>
         <v>0</v>
       </c>
-      <c r="I23" s="112" t="s">
+      <c r="I23" s="131" t="s">
         <v>56</v>
       </c>
-      <c r="J23" s="112"/>
-      <c r="K23" s="112"/>
-      <c r="L23" s="112"/>
+      <c r="J23" s="131"/>
+      <c r="K23" s="131"/>
+      <c r="L23" s="131"/>
       <c r="M23" s="23">
         <f>M22/60</f>
         <v>122.5</v>
@@ -2317,7 +2323,7 @@
       </c>
     </row>
     <row r="24" spans="2:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="122"/>
+      <c r="B24" s="120"/>
       <c r="C24" s="7" t="s">
         <v>16</v>
       </c>
@@ -2335,12 +2341,12 @@
         <f>(F24/60)*Estimación!$J$15</f>
         <v>832.41666666666663</v>
       </c>
-      <c r="I24" s="112" t="s">
+      <c r="I24" s="131" t="s">
         <v>57</v>
       </c>
-      <c r="J24" s="112"/>
-      <c r="K24" s="112"/>
-      <c r="L24" s="112"/>
+      <c r="J24" s="131"/>
+      <c r="K24" s="131"/>
+      <c r="L24" s="131"/>
       <c r="M24" s="24">
         <f>M23*Estimación!J15</f>
         <v>5098.552083333333</v>
@@ -2394,6 +2400,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I24:L24"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D13:D14"/>
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="B4:K5"/>
     <mergeCell ref="B19:B20"/>
@@ -2410,22 +2432,6 @@
     <mergeCell ref="I21:K21"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I24:L24"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="58" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2803,23 +2809,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G2" s="96" t="s">
+      <c r="G2" s="99" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="96"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="96"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
     </row>
     <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="161"/>
-      <c r="C4" s="159" t="s">
+      <c r="B4" s="141"/>
+      <c r="C4" s="139" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="160"/>
-      <c r="E4" s="160"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
     </row>
     <row r="5" spans="2:10" ht="36.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="162"/>
+      <c r="B5" s="142"/>
       <c r="C5" s="70" t="s">
         <v>74</v>
       </c>
@@ -2831,7 +2837,7 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="142" t="s">
+      <c r="B6" s="143" t="s">
         <v>78</v>
       </c>
       <c r="C6" s="50">
@@ -2839,14 +2845,14 @@
       </c>
       <c r="D6" s="71"/>
       <c r="E6" s="71"/>
-      <c r="G6" s="158" t="s">
+      <c r="G6" s="138" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="158"/>
-      <c r="I6" s="158"/>
+      <c r="H6" s="138"/>
+      <c r="I6" s="138"/>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="142"/>
+      <c r="B7" s="143"/>
       <c r="C7" s="71"/>
       <c r="D7" s="50">
         <v>1</v>
@@ -2857,18 +2863,18 @@
       <c r="I7" s="32"/>
     </row>
     <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="142"/>
+      <c r="B8" s="143"/>
       <c r="C8" s="71"/>
       <c r="D8" s="71"/>
       <c r="E8" s="50">
         <v>2</v>
       </c>
-      <c r="G8" s="146"/>
+      <c r="G8" s="145"/>
       <c r="H8" s="34"/>
       <c r="I8" s="51"/>
     </row>
     <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="141" t="s">
+      <c r="B9" s="161" t="s">
         <v>79</v>
       </c>
       <c r="C9" s="50">
@@ -2876,68 +2882,68 @@
       </c>
       <c r="D9" s="71"/>
       <c r="E9" s="71"/>
-      <c r="G9" s="146"/>
+      <c r="G9" s="145"/>
       <c r="H9" s="38"/>
       <c r="I9" s="51"/>
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="142"/>
+      <c r="B10" s="143"/>
       <c r="C10" s="71"/>
       <c r="D10" s="50">
         <v>2</v>
       </c>
       <c r="E10" s="71"/>
-      <c r="G10" s="146"/>
+      <c r="G10" s="145"/>
       <c r="H10" s="34"/>
       <c r="I10" s="51"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="143"/>
+      <c r="B11" s="162"/>
       <c r="C11" s="71"/>
       <c r="D11" s="71"/>
       <c r="E11" s="50">
         <v>3</v>
       </c>
-      <c r="G11" s="146"/>
+      <c r="G11" s="145"/>
       <c r="H11" s="38"/>
       <c r="I11" s="51"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G12" s="146"/>
+      <c r="G12" s="145"/>
       <c r="H12" s="38"/>
       <c r="I12" s="51"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G13" s="146"/>
+      <c r="G13" s="145"/>
       <c r="H13" s="34"/>
       <c r="I13" s="51"/>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G14" s="146"/>
+      <c r="G14" s="145"/>
       <c r="H14" s="38"/>
       <c r="I14" s="30"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="150" t="s">
+      <c r="B15" s="153" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="150"/>
-      <c r="D15" s="150"/>
-      <c r="E15" s="151" t="s">
+      <c r="C15" s="153"/>
+      <c r="D15" s="153"/>
+      <c r="E15" s="155" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="151"/>
-      <c r="G15" s="151"/>
-      <c r="H15" s="151" t="s">
+      <c r="F15" s="155"/>
+      <c r="G15" s="155"/>
+      <c r="H15" s="155" t="s">
         <v>83</v>
       </c>
-      <c r="I15" s="151"/>
-      <c r="J15" s="151"/>
+      <c r="I15" s="155"/>
+      <c r="J15" s="155"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="150"/>
-      <c r="C16" s="150"/>
-      <c r="D16" s="150"/>
+      <c r="B16" s="153"/>
+      <c r="C16" s="153"/>
+      <c r="D16" s="153"/>
       <c r="E16" s="78" t="s">
         <v>84</v>
       </c>
@@ -2958,27 +2964,27 @@
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="145" t="s">
+      <c r="B17" s="154" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="145"/>
-      <c r="D17" s="145"/>
-      <c r="E17" s="144">
+      <c r="C17" s="154"/>
+      <c r="D17" s="154"/>
+      <c r="E17" s="146">
         <v>0.16</v>
       </c>
-      <c r="F17" s="144">
+      <c r="F17" s="146">
         <v>0.16</v>
       </c>
-      <c r="G17" s="144">
+      <c r="G17" s="146">
         <v>0.16</v>
       </c>
-      <c r="H17" s="144">
+      <c r="H17" s="146">
         <v>0.16</v>
       </c>
-      <c r="I17" s="144">
+      <c r="I17" s="146">
         <v>0.16</v>
       </c>
-      <c r="J17" s="144">
+      <c r="J17" s="146">
         <v>0.16</v>
       </c>
       <c r="K17" s="30"/>
@@ -2991,17 +2997,17 @@
       <c r="R17" s="30"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="145" t="s">
+      <c r="B18" s="154" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="145"/>
-      <c r="D18" s="145"/>
-      <c r="E18" s="144"/>
-      <c r="F18" s="144"/>
-      <c r="G18" s="144"/>
-      <c r="H18" s="144"/>
-      <c r="I18" s="144"/>
-      <c r="J18" s="144"/>
+      <c r="C18" s="154"/>
+      <c r="D18" s="154"/>
+      <c r="E18" s="146"/>
+      <c r="F18" s="146"/>
+      <c r="G18" s="146"/>
+      <c r="H18" s="146"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="146"/>
       <c r="K18" s="30"/>
       <c r="L18" s="30"/>
       <c r="M18" s="30"/>
@@ -3012,65 +3018,65 @@
       <c r="R18" s="30"/>
     </row>
     <row r="19" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="145" t="s">
+      <c r="B19" s="154" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="145"/>
-      <c r="D19" s="145"/>
-      <c r="E19" s="144">
+      <c r="C19" s="154"/>
+      <c r="D19" s="154"/>
+      <c r="E19" s="146">
         <v>0.25</v>
       </c>
-      <c r="F19" s="144">
+      <c r="F19" s="146">
         <v>0.25</v>
       </c>
-      <c r="G19" s="144">
+      <c r="G19" s="146">
         <v>0.25</v>
       </c>
-      <c r="H19" s="144">
+      <c r="H19" s="146">
         <v>0.25</v>
       </c>
-      <c r="I19" s="144">
+      <c r="I19" s="146">
         <v>0.25</v>
       </c>
-      <c r="J19" s="144">
+      <c r="J19" s="146">
         <v>0.25</v>
       </c>
-      <c r="K19" s="149"/>
-      <c r="L19" s="149"/>
-      <c r="M19" s="149"/>
+      <c r="K19" s="159"/>
+      <c r="L19" s="159"/>
+      <c r="M19" s="159"/>
       <c r="N19" s="60"/>
       <c r="O19" s="60"/>
       <c r="P19" s="60"/>
-      <c r="Q19" s="147"/>
+      <c r="Q19" s="156"/>
       <c r="R19" s="30"/>
     </row>
     <row r="20" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="145" t="s">
+      <c r="B20" s="154" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="145"/>
-      <c r="D20" s="145"/>
-      <c r="E20" s="144"/>
-      <c r="F20" s="144"/>
-      <c r="G20" s="144"/>
-      <c r="H20" s="144"/>
-      <c r="I20" s="144"/>
-      <c r="J20" s="144"/>
-      <c r="K20" s="149"/>
-      <c r="L20" s="149"/>
-      <c r="M20" s="149"/>
+      <c r="C20" s="154"/>
+      <c r="D20" s="154"/>
+      <c r="E20" s="146"/>
+      <c r="F20" s="146"/>
+      <c r="G20" s="146"/>
+      <c r="H20" s="146"/>
+      <c r="I20" s="146"/>
+      <c r="J20" s="146"/>
+      <c r="K20" s="159"/>
+      <c r="L20" s="159"/>
+      <c r="M20" s="159"/>
       <c r="N20" s="60"/>
       <c r="O20" s="60"/>
       <c r="P20" s="60"/>
-      <c r="Q20" s="147"/>
+      <c r="Q20" s="156"/>
       <c r="R20" s="30"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="155" t="s">
+      <c r="B21" s="150" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="156"/>
-      <c r="D21" s="157"/>
+      <c r="C21" s="151"/>
+      <c r="D21" s="152"/>
       <c r="E21" s="47">
         <v>0.16</v>
       </c>
@@ -3089,21 +3095,21 @@
       <c r="J21" s="47">
         <v>0.16</v>
       </c>
-      <c r="K21" s="140"/>
-      <c r="L21" s="140"/>
-      <c r="M21" s="140"/>
+      <c r="K21" s="157"/>
+      <c r="L21" s="157"/>
+      <c r="M21" s="157"/>
       <c r="N21" s="55"/>
       <c r="O21" s="55"/>
       <c r="P21" s="55"/>
-      <c r="Q21" s="148"/>
+      <c r="Q21" s="158"/>
       <c r="R21" s="54"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="145" t="s">
+      <c r="B22" s="154" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="145"/>
-      <c r="D22" s="145"/>
+      <c r="C22" s="154"/>
+      <c r="D22" s="154"/>
       <c r="E22" s="79">
         <f>Servicios!C9</f>
         <v>1</v>
@@ -3128,21 +3134,21 @@
         <f>Servicios!E8</f>
         <v>2</v>
       </c>
-      <c r="K22" s="140"/>
-      <c r="L22" s="140"/>
-      <c r="M22" s="140"/>
+      <c r="K22" s="157"/>
+      <c r="L22" s="157"/>
+      <c r="M22" s="157"/>
       <c r="N22" s="55"/>
       <c r="O22" s="55"/>
       <c r="P22" s="55"/>
-      <c r="Q22" s="148"/>
+      <c r="Q22" s="158"/>
       <c r="R22" s="54"/>
     </row>
     <row r="23" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="152" t="s">
+      <c r="B23" s="147" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="153"/>
-      <c r="D23" s="154"/>
+      <c r="C23" s="148"/>
+      <c r="D23" s="149"/>
       <c r="E23" s="82">
         <f t="shared" ref="E23:J23" si="0">SUM(E17:E22)</f>
         <v>1.57</v>
@@ -3167,9 +3173,9 @@
         <f t="shared" si="0"/>
         <v>2.5700000000000003</v>
       </c>
-      <c r="K23" s="140"/>
-      <c r="L23" s="140"/>
-      <c r="M23" s="140"/>
+      <c r="K23" s="157"/>
+      <c r="L23" s="157"/>
+      <c r="M23" s="157"/>
       <c r="N23" s="55"/>
       <c r="O23" s="55"/>
       <c r="P23" s="55"/>
@@ -3182,9 +3188,9 @@
       <c r="H24" s="38"/>
       <c r="I24" s="51"/>
       <c r="J24" s="32"/>
-      <c r="K24" s="140"/>
-      <c r="L24" s="140"/>
-      <c r="M24" s="140"/>
+      <c r="K24" s="157"/>
+      <c r="L24" s="157"/>
+      <c r="M24" s="157"/>
       <c r="N24" s="55"/>
       <c r="O24" s="55"/>
       <c r="P24" s="55"/>
@@ -3193,58 +3199,58 @@
     </row>
     <row r="25" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F25" s="30"/>
-      <c r="G25" s="146"/>
+      <c r="G25" s="145"/>
       <c r="H25" s="34"/>
       <c r="I25" s="51"/>
       <c r="J25" s="33"/>
-      <c r="K25" s="140"/>
-      <c r="L25" s="140"/>
-      <c r="M25" s="140"/>
+      <c r="K25" s="157"/>
+      <c r="L25" s="157"/>
+      <c r="M25" s="157"/>
       <c r="N25" s="55"/>
       <c r="O25" s="55"/>
       <c r="P25" s="55"/>
-      <c r="Q25" s="148"/>
+      <c r="Q25" s="158"/>
       <c r="R25" s="54"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F26" s="30"/>
-      <c r="G26" s="146"/>
+      <c r="G26" s="145"/>
       <c r="H26" s="38"/>
       <c r="I26" s="51"/>
       <c r="J26" s="33"/>
-      <c r="K26" s="140"/>
-      <c r="L26" s="140"/>
-      <c r="M26" s="140"/>
+      <c r="K26" s="157"/>
+      <c r="L26" s="157"/>
+      <c r="M26" s="157"/>
       <c r="N26" s="55"/>
       <c r="O26" s="55"/>
       <c r="P26" s="55"/>
-      <c r="Q26" s="148"/>
+      <c r="Q26" s="158"/>
       <c r="R26" s="54"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F27" s="30"/>
-      <c r="G27" s="146"/>
+      <c r="G27" s="145"/>
       <c r="H27" s="34"/>
       <c r="I27" s="51"/>
       <c r="J27" s="33"/>
-      <c r="K27" s="140"/>
-      <c r="L27" s="140"/>
-      <c r="M27" s="140"/>
+      <c r="K27" s="157"/>
+      <c r="L27" s="157"/>
+      <c r="M27" s="157"/>
       <c r="N27" s="55"/>
       <c r="O27" s="55"/>
       <c r="P27" s="55"/>
-      <c r="Q27" s="148"/>
+      <c r="Q27" s="158"/>
       <c r="R27" s="54"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F28" s="30"/>
-      <c r="G28" s="146"/>
+      <c r="G28" s="145"/>
       <c r="H28" s="38"/>
       <c r="I28" s="51"/>
       <c r="J28" s="33"/>
-      <c r="K28" s="140"/>
-      <c r="L28" s="140"/>
-      <c r="M28" s="140"/>
+      <c r="K28" s="157"/>
+      <c r="L28" s="157"/>
+      <c r="M28" s="157"/>
       <c r="N28" s="55"/>
       <c r="O28" s="55"/>
       <c r="P28" s="55"/>
@@ -3253,13 +3259,13 @@
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F29" s="30"/>
-      <c r="G29" s="138"/>
-      <c r="H29" s="138"/>
+      <c r="G29" s="144"/>
+      <c r="H29" s="144"/>
       <c r="I29" s="51"/>
       <c r="J29" s="33"/>
-      <c r="K29" s="140"/>
-      <c r="L29" s="140"/>
-      <c r="M29" s="140"/>
+      <c r="K29" s="157"/>
+      <c r="L29" s="157"/>
+      <c r="M29" s="157"/>
       <c r="N29" s="55"/>
       <c r="O29" s="55"/>
       <c r="P29" s="55"/>
@@ -3268,13 +3274,13 @@
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F30" s="30"/>
-      <c r="G30" s="138"/>
-      <c r="H30" s="138"/>
+      <c r="G30" s="144"/>
+      <c r="H30" s="144"/>
       <c r="I30" s="53"/>
       <c r="J30" s="33"/>
-      <c r="K30" s="138"/>
-      <c r="L30" s="138"/>
-      <c r="M30" s="138"/>
+      <c r="K30" s="144"/>
+      <c r="L30" s="144"/>
+      <c r="M30" s="144"/>
       <c r="N30" s="56"/>
       <c r="O30" s="56"/>
       <c r="P30" s="56"/>
@@ -3287,12 +3293,12 @@
       <c r="H31" s="31"/>
       <c r="I31" s="34"/>
       <c r="J31" s="33"/>
-      <c r="K31" s="139"/>
-      <c r="L31" s="139"/>
-      <c r="M31" s="139"/>
-      <c r="N31" s="139"/>
-      <c r="O31" s="139"/>
-      <c r="P31" s="139"/>
+      <c r="K31" s="160"/>
+      <c r="L31" s="160"/>
+      <c r="M31" s="160"/>
+      <c r="N31" s="160"/>
+      <c r="O31" s="160"/>
+      <c r="P31" s="160"/>
       <c r="Q31" s="57"/>
       <c r="R31" s="58"/>
     </row>
@@ -3302,12 +3308,12 @@
       <c r="H32" s="31"/>
       <c r="I32" s="38"/>
       <c r="J32" s="33"/>
-      <c r="K32" s="139"/>
-      <c r="L32" s="139"/>
-      <c r="M32" s="139"/>
-      <c r="N32" s="139"/>
-      <c r="O32" s="139"/>
-      <c r="P32" s="139"/>
+      <c r="K32" s="160"/>
+      <c r="L32" s="160"/>
+      <c r="M32" s="160"/>
+      <c r="N32" s="160"/>
+      <c r="O32" s="160"/>
+      <c r="P32" s="160"/>
       <c r="Q32" s="59"/>
       <c r="R32" s="30"/>
     </row>
@@ -3343,38 +3349,6 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="G29:H30"/>
-    <mergeCell ref="G25:G28"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="B15:D16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="Q25:Q27"/>
-    <mergeCell ref="K19:M20"/>
-    <mergeCell ref="Q21:Q22"/>
     <mergeCell ref="K30:M30"/>
     <mergeCell ref="K31:P31"/>
     <mergeCell ref="K32:P32"/>
@@ -3391,6 +3365,38 @@
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="G8:G11"/>
     <mergeCell ref="J17:J18"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="Q25:Q27"/>
+    <mergeCell ref="K19:M20"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="B15:D16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="G29:H30"/>
+    <mergeCell ref="G25:G28"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3438,27 +3444,27 @@
       </c>
       <c r="G2" s="163"/>
       <c r="H2" s="84" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="84" t="s">
         <v>98</v>
       </c>
-      <c r="I2" s="84" t="s">
-        <v>99</v>
-      </c>
       <c r="J2" s="84" t="s">
-        <v>121</v>
-      </c>
-      <c r="K2" s="158" t="s">
+        <v>120</v>
+      </c>
+      <c r="K2" s="138" t="s">
+        <v>100</v>
+      </c>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
+      <c r="O2" s="138"/>
+      <c r="P2" s="138"/>
+      <c r="Q2" s="84" t="s">
         <v>101</v>
       </c>
-      <c r="L2" s="158"/>
-      <c r="M2" s="158"/>
-      <c r="N2" s="158"/>
-      <c r="O2" s="158"/>
-      <c r="P2" s="158"/>
-      <c r="Q2" s="84" t="s">
-        <v>102</v>
-      </c>
       <c r="R2" s="84" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -3489,7 +3495,7 @@
       </c>
       <c r="L3" s="164"/>
       <c r="M3" s="164" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N3" s="164"/>
       <c r="O3" s="164" t="s">
@@ -3567,7 +3573,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="85" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" s="67">
         <v>2</v>
@@ -3639,16 +3645,16 @@
     <row r="9" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="83"/>
       <c r="B9" s="84" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="83"/>
       <c r="D9" s="84" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="86" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" s="72">
         <v>1</v>
@@ -3661,7 +3667,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="85" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" s="72">
         <v>2</v>
@@ -3674,7 +3680,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="85" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B12" s="72">
         <v>0.5</v>
@@ -3733,31 +3739,31 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="90" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="90" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="90" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" s="92" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="90" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="89" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="66"/>
       <c r="C7" s="66"/>
@@ -3775,29 +3781,29 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="90" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B9" s="90" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" s="90" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="90" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B10" s="90" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" s="90" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="90" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualizacion del plan de estimacion
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Planeacion/Estimación-150204.xlsx
+++ b/qualtcom/Procesos/Planeacion/Estimación-150204.xlsx
@@ -19,7 +19,7 @@
     <sheet name="Capacidad" sheetId="5" r:id="rId5"/>
     <sheet name="Tipo" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -52,6 +52,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
+    <author>zepeda</author>
   </authors>
   <commentList>
     <comment ref="J2" authorId="0" shapeId="0">
@@ -69,6 +70,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="K2" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Obtencion de datos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+La primer columna nace por la sumatoria de las etapas de los servicios con excepcion de esfuerzo de obra.
+La segunda columna surge como la multiplicacion de la  sumatoria de esfuerzo por los servicios al dia y finalmente por los dias laborales por mes promedio
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -515,7 +542,7 @@
     <numFmt numFmtId="165" formatCode="_-[$$-80A]* #,##0.00_-;\-[$$-80A]* #,##0.00_-;_-[$$-80A]* \-??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -600,6 +627,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -774,48 +814,6 @@
   </cellStyleXfs>
   <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -994,78 +992,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1074,9 +1000,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1086,6 +1009,123 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1554,252 +1594,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
+      <c r="C1" s="87"/>
     </row>
     <row r="5" spans="2:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="I5" s="12" t="s">
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="I5" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
     </row>
     <row r="6" spans="2:11" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="21" t="s">
+      <c r="J6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="23">
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="9">
         <f>Capacidad!J5</f>
         <v>720</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="9">
         <f>Capacidad!J4</f>
         <v>1920</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="10">
         <f>(E7+F7)*$J$15</f>
         <v>109878.99999999999</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="12">
         <v>9000</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="12">
         <v>15000</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="23">
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="9">
         <f>Capacidad!R5</f>
         <v>547.20000000000005</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="9">
         <f>Capacidad!R4</f>
         <v>1094.4000000000001</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="10">
         <f>(E8+F8)*$J$15</f>
         <v>68324.759999999995</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J8" s="12">
         <v>250</v>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="12">
         <v>250</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="10">
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="86">
         <f>Capacidad!D10</f>
         <v>12</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="24">
+      <c r="F9" s="86"/>
+      <c r="G9" s="10">
         <f>+E9*$K$15</f>
         <v>799.45</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="12">
         <v>100</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="12">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="10">
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="86">
         <f>Capacidad!D11</f>
         <v>24</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="24">
+      <c r="F10" s="86"/>
+      <c r="G10" s="10">
         <f>+E10*$J$15</f>
         <v>998.89999999999986</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="84">
         <v>389</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="84">
         <v>389</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="10">
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="86">
         <f>Capacidad!D12</f>
         <v>6</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="24">
+      <c r="F11" s="86"/>
+      <c r="G11" s="10">
         <f>+E11*$J$15</f>
         <v>249.72499999999997</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="84"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="24"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="10"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
     </row>
     <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="7">
+      <c r="C13" s="82"/>
+      <c r="D13" s="82"/>
+      <c r="E13" s="83">
         <f>SUM(E7:F12)</f>
         <v>4323.6000000000004</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="29">
+      <c r="F13" s="83"/>
+      <c r="G13" s="15">
         <f>SUM(G7:G12)</f>
         <v>180251.83499999999</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="26">
+      <c r="J13" s="12">
         <v>250</v>
       </c>
-      <c r="K13" s="26">
+      <c r="K13" s="12">
         <v>250</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I14" s="30" t="s">
+      <c r="I14" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J14" s="17">
         <f>SUM(J7:J13)</f>
         <v>9989</v>
       </c>
-      <c r="K14" s="31">
+      <c r="K14" s="17">
         <f>SUM(K7:K13)</f>
         <v>15989</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I15" s="32" t="s">
+      <c r="I15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="31">
+      <c r="J15" s="17">
         <f>(J14/30)/8</f>
         <v>41.62083333333333</v>
       </c>
-      <c r="K15" s="31">
+      <c r="K15" s="17">
         <f>(K14/30)/8</f>
         <v>66.620833333333337</v>
       </c>
     </row>
     <row r="27" spans="13:16" x14ac:dyDescent="0.25">
-      <c r="M27" s="33">
+      <c r="M27" s="19">
         <f>SUM(Servicios!E23:G23)</f>
         <v>7.7100000000000009</v>
       </c>
-      <c r="P27" s="33">
+      <c r="P27" s="19">
         <f>SUM(Servicios!H23:J23)</f>
-        <v>5.2100000000000009</v>
+        <v>4.7100000000000009</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="J10:J11"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="K10:K11"/>
@@ -1807,16 +1857,6 @@
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1845,580 +1885,559 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="20" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="100"/>
     </row>
     <row r="6" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3" t="s">
+      <c r="F6" s="103"/>
+      <c r="G6" s="103"/>
+      <c r="H6" s="103"/>
+      <c r="I6" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="5" t="s">
+      <c r="J6" s="103"/>
+      <c r="K6" s="101" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5" t="s">
+      <c r="B7" s="101"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5" t="s">
+      <c r="H7" s="101"/>
+      <c r="I7" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="35" t="s">
+      <c r="B8" s="101"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="5"/>
+      <c r="K8" s="101"/>
     </row>
     <row r="9" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="95" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="95">
         <v>30</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="22">
         <v>30</v>
       </c>
-      <c r="F9" s="37"/>
-      <c r="G9" s="20">
+      <c r="F9" s="23"/>
+      <c r="G9" s="6">
         <v>30</v>
       </c>
-      <c r="H9" s="37"/>
-      <c r="I9" s="36">
+      <c r="H9" s="23"/>
+      <c r="I9" s="22">
         <v>10</v>
       </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="20">
+      <c r="J9" s="23"/>
+      <c r="K9" s="6">
         <f>I9+G9+E9+$D$9</f>
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="95"/>
+      <c r="C10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="36">
+      <c r="D10" s="95"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="22">
         <v>60</v>
       </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="20">
+      <c r="G10" s="23"/>
+      <c r="H10" s="6">
         <v>60</v>
       </c>
-      <c r="I10" s="38"/>
-      <c r="J10" s="36">
+      <c r="I10" s="24"/>
+      <c r="J10" s="22">
         <v>60</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="6">
         <f>J10+H10+F10+$D$9</f>
         <v>210</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="95">
         <v>45</v>
       </c>
-      <c r="E11" s="36">
+      <c r="E11" s="22">
         <v>30</v>
       </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="20">
+      <c r="F11" s="23"/>
+      <c r="G11" s="6">
         <v>30</v>
       </c>
-      <c r="H11" s="37"/>
-      <c r="I11" s="36">
+      <c r="H11" s="23"/>
+      <c r="I11" s="22">
         <v>10</v>
       </c>
-      <c r="J11" s="37"/>
-      <c r="K11" s="20">
+      <c r="J11" s="23"/>
+      <c r="K11" s="6">
         <f>I11+G11+E11+$D$11</f>
         <v>115</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="95"/>
+      <c r="C12" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="36">
+      <c r="D12" s="95"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="22">
         <v>60</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="20">
+      <c r="G12" s="23"/>
+      <c r="H12" s="6">
         <v>60</v>
       </c>
-      <c r="I12" s="38"/>
-      <c r="J12" s="36">
+      <c r="I12" s="24"/>
+      <c r="J12" s="22">
         <v>60</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K12" s="6">
         <f>J12+H12+F12+$D$11</f>
         <v>225</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="95">
         <v>90</v>
       </c>
-      <c r="E13" s="36">
+      <c r="E13" s="22">
         <v>30</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="20">
+      <c r="F13" s="24"/>
+      <c r="G13" s="6">
         <v>30</v>
       </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="36">
+      <c r="H13" s="23"/>
+      <c r="I13" s="22">
         <v>30</v>
       </c>
-      <c r="J13" s="38"/>
-      <c r="K13" s="20">
+      <c r="J13" s="24"/>
+      <c r="K13" s="6">
         <f>I13+G13+E13+D13</f>
         <v>180</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="90"/>
+      <c r="C14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="36">
+      <c r="D14" s="95"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="22">
         <v>90</v>
       </c>
-      <c r="G14" s="37"/>
-      <c r="H14" s="20">
+      <c r="G14" s="23"/>
+      <c r="H14" s="6">
         <v>60</v>
       </c>
-      <c r="I14" s="38"/>
-      <c r="J14" s="36">
+      <c r="I14" s="24"/>
+      <c r="J14" s="22">
         <v>60</v>
       </c>
-      <c r="K14" s="20">
+      <c r="K14" s="6">
         <f>J14+H14+F14+D13</f>
         <v>300</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="89" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="89"/>
-      <c r="I15" s="89"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="97"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="97"/>
+      <c r="J15" s="97"/>
+      <c r="K15" s="97"/>
     </row>
     <row r="17" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="90" t="s">
+      <c r="B17" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="90"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="90"/>
-      <c r="F17" s="90"/>
-      <c r="G17" s="90"/>
-      <c r="I17" s="90" t="s">
+      <c r="C17" s="98"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="98"/>
+      <c r="I17" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="90"/>
-      <c r="K17" s="90"/>
-      <c r="L17" s="35" t="s">
+      <c r="J17" s="98"/>
+      <c r="K17" s="98"/>
+      <c r="L17" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="M17" s="35" t="s">
+      <c r="M17" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="N17" s="41"/>
+      <c r="N17" s="27"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="42" t="s">
+      <c r="F18" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="42" t="s">
+      <c r="G18" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="I18" s="91" t="s">
+      <c r="I18" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="91"/>
-      <c r="K18" s="91"/>
-      <c r="L18" s="92">
+      <c r="J18" s="94"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="99">
         <v>15</v>
       </c>
-      <c r="M18" s="93">
+      <c r="M18" s="92">
         <f>L18*$E$25</f>
         <v>765</v>
       </c>
-      <c r="N18" s="41"/>
+      <c r="N18" s="27"/>
     </row>
     <row r="19" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="6">
         <v>10</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="6">
         <f>D19*1.5</f>
         <v>15</v>
       </c>
-      <c r="F19" s="43">
+      <c r="F19" s="29">
         <f t="shared" ref="F19:F24" si="0">E19*K9</f>
         <v>1500</v>
       </c>
-      <c r="G19" s="45">
+      <c r="G19" s="31">
         <f>(F19/60)*Estimación!$J$15</f>
         <v>1040.5208333333333</v>
       </c>
-      <c r="I19" s="91" t="s">
+      <c r="I19" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="J19" s="91"/>
-      <c r="K19" s="91"/>
-      <c r="L19" s="92"/>
-      <c r="M19" s="93"/>
-      <c r="N19" s="41"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="94"/>
+      <c r="L19" s="99"/>
+      <c r="M19" s="92"/>
+      <c r="N19" s="27"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="94"/>
-      <c r="C20" s="22" t="s">
+      <c r="B20" s="93"/>
+      <c r="C20" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="6">
         <v>0</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="6">
         <v>1</v>
       </c>
-      <c r="F20" s="43">
+      <c r="F20" s="29">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
-      <c r="G20" s="45">
+      <c r="G20" s="31">
         <f>(F20/60)*Estimación!$J$15</f>
         <v>145.67291666666665</v>
       </c>
-      <c r="I20" s="91" t="s">
+      <c r="I20" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="J20" s="91"/>
-      <c r="K20" s="91"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="43">
+      <c r="J20" s="94"/>
+      <c r="K20" s="94"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="29">
         <f>F25</f>
         <v>6585</v>
       </c>
-      <c r="N20" s="41"/>
+      <c r="N20" s="27"/>
     </row>
     <row r="21" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="6">
         <v>20</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="6">
         <f>D21*1.5</f>
         <v>30</v>
       </c>
-      <c r="F21" s="43">
+      <c r="F21" s="29">
         <f t="shared" si="0"/>
         <v>3450</v>
       </c>
-      <c r="G21" s="45">
+      <c r="G21" s="31">
         <f>(F21/60)*Estimación!$J$15</f>
         <v>2393.1979166666665</v>
       </c>
-      <c r="I21" s="91" t="s">
+      <c r="I21" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="91"/>
-      <c r="K21" s="91"/>
-      <c r="L21" s="43">
+      <c r="J21" s="94"/>
+      <c r="K21" s="94"/>
+      <c r="L21" s="29">
         <v>10</v>
       </c>
-      <c r="M21" s="20">
+      <c r="M21" s="6">
         <f>L21*$E$25</f>
         <v>510</v>
       </c>
-      <c r="N21" s="41"/>
+      <c r="N21" s="27"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="22" t="s">
+      <c r="B22" s="95"/>
+      <c r="C22" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="6">
         <v>0</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="6">
         <v>1</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F22" s="29">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
-      <c r="G22" s="45">
+      <c r="G22" s="31">
         <f>(F22/60)*Estimación!$J$15</f>
         <v>156.078125</v>
       </c>
-      <c r="I22" s="95" t="s">
+      <c r="I22" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="95"/>
-      <c r="K22" s="95"/>
-      <c r="L22" s="43">
+      <c r="J22" s="96"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="29">
         <f>SUM(L18:L21)</f>
         <v>25</v>
       </c>
-      <c r="M22" s="43">
+      <c r="M22" s="29">
         <f>SUM(M18:M20)</f>
         <v>7350</v>
       </c>
-      <c r="N22" s="41"/>
+      <c r="N22" s="27"/>
     </row>
     <row r="23" spans="2:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="6">
         <v>0</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="6">
         <f>D23*1.5</f>
         <v>0</v>
       </c>
-      <c r="F23" s="43">
+      <c r="F23" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="45">
+      <c r="G23" s="31">
         <f>(F23/60)*Estimación!$J$15</f>
         <v>0</v>
       </c>
-      <c r="I23" s="96" t="s">
+      <c r="I23" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="J23" s="96"/>
-      <c r="K23" s="96"/>
-      <c r="L23" s="96"/>
-      <c r="M23" s="47">
+      <c r="J23" s="91"/>
+      <c r="K23" s="91"/>
+      <c r="L23" s="91"/>
+      <c r="M23" s="33">
         <f>M22/60</f>
         <v>122.5</v>
       </c>
-      <c r="N23" s="48" t="s">
+      <c r="N23" s="34" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
-      <c r="C24" s="22" t="s">
+      <c r="B24" s="90"/>
+      <c r="C24" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="6">
         <v>0</v>
       </c>
-      <c r="E24" s="20">
+      <c r="E24" s="6">
         <v>4</v>
       </c>
-      <c r="F24" s="43">
+      <c r="F24" s="29">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-      <c r="G24" s="45">
+      <c r="G24" s="31">
         <f>(F24/60)*Estimación!$J$15</f>
         <v>832.41666666666663</v>
       </c>
-      <c r="I24" s="96" t="s">
+      <c r="I24" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="J24" s="96"/>
-      <c r="K24" s="96"/>
-      <c r="L24" s="96"/>
-      <c r="M24" s="49">
+      <c r="J24" s="91"/>
+      <c r="K24" s="91"/>
+      <c r="L24" s="91"/>
+      <c r="M24" s="35">
         <f>M23*Estimación!J15</f>
         <v>5098.552083333333</v>
       </c>
-      <c r="N24" s="41"/>
+      <c r="N24" s="27"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="50" t="s">
+      <c r="C25" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D25" s="6">
         <f>SUM(D19:D24)</f>
         <v>30</v>
       </c>
-      <c r="E25" s="20">
+      <c r="E25" s="6">
         <f>SUM(E19:E24)</f>
         <v>51</v>
       </c>
-      <c r="F25" s="43">
+      <c r="F25" s="29">
         <f>SUM(F19:F24)</f>
         <v>6585</v>
       </c>
-      <c r="G25" s="51">
+      <c r="G25" s="37">
         <f>SUM(G19:G24)</f>
         <v>4567.8864583333334</v>
       </c>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="52"/>
-      <c r="M25" s="53"/>
-      <c r="N25" s="41"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="39"/>
+      <c r="N25" s="27"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I26" s="41"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="41"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="40"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="27"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I29" s="56"/>
-      <c r="J29" s="57"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="I24:L24"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D13:D14"/>
     <mergeCell ref="B4:K5"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="C6:C8"/>
@@ -2430,6 +2449,27 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="I24:L24"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
   </mergeCells>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2780,30 +2820,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK23"/>
   <sheetViews>
-    <sheetView topLeftCell="E6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="33"/>
-    <col min="2" max="2" width="17.42578125" style="33"/>
-    <col min="3" max="3" width="5.5703125" style="33"/>
-    <col min="4" max="5" width="6.5703125" style="33"/>
-    <col min="6" max="6" width="7.140625" style="33"/>
-    <col min="7" max="7" width="24.28515625" style="33"/>
-    <col min="8" max="8" width="16" style="33"/>
-    <col min="9" max="9" width="14.28515625" style="33"/>
-    <col min="10" max="10" width="7.140625" style="33"/>
-    <col min="11" max="13" width="14.28515625" style="33"/>
-    <col min="14" max="14" width="7.42578125" style="33"/>
-    <col min="15" max="15" width="8" style="33"/>
-    <col min="16" max="16" width="7.28515625" style="33"/>
-    <col min="17" max="17" width="7.7109375" style="33"/>
-    <col min="18" max="18" width="8.5703125" style="33"/>
-    <col min="19" max="19" width="7.85546875" style="33"/>
-    <col min="20" max="63" width="14.28515625" style="33"/>
-    <col min="64" max="1025" width="11.42578125" style="33"/>
+    <col min="1" max="1" width="2.85546875" style="19"/>
+    <col min="2" max="2" width="17.42578125" style="19"/>
+    <col min="3" max="3" width="5.5703125" style="19"/>
+    <col min="4" max="5" width="6.5703125" style="19"/>
+    <col min="6" max="6" width="7.140625" style="19"/>
+    <col min="7" max="7" width="24.28515625" style="19"/>
+    <col min="8" max="8" width="16" style="19"/>
+    <col min="9" max="9" width="14.28515625" style="19"/>
+    <col min="10" max="10" width="7.140625" style="19"/>
+    <col min="11" max="13" width="14.28515625" style="19"/>
+    <col min="14" max="14" width="7.42578125" style="19"/>
+    <col min="15" max="15" width="8" style="19"/>
+    <col min="16" max="16" width="7.28515625" style="19"/>
+    <col min="17" max="17" width="7.7109375" style="19"/>
+    <col min="18" max="18" width="8.5703125" style="19"/>
+    <col min="19" max="19" width="7.85546875" style="19"/>
+    <col min="20" max="63" width="14.28515625" style="19"/>
+    <col min="64" max="1025" width="11.42578125" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
@@ -2831,12 +2871,12 @@
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
@@ -2866,12 +2906,12 @@
       <c r="R3"/>
     </row>
     <row r="4" spans="2:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="97"/>
-      <c r="C4" s="98" t="s">
+      <c r="B4" s="114"/>
+      <c r="C4" s="115" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
@@ -2887,14 +2927,14 @@
       <c r="R4"/>
     </row>
     <row r="5" spans="2:18" ht="36.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="97"/>
-      <c r="C5" s="58" t="s">
+      <c r="B5" s="114"/>
+      <c r="C5" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="45" t="s">
         <v>84</v>
       </c>
       <c r="F5"/>
@@ -2912,20 +2952,20 @@
       <c r="R5"/>
     </row>
     <row r="6" spans="2:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="99" t="s">
+      <c r="B6" s="116" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="60">
+      <c r="C6" s="46">
         <v>0.5</v>
       </c>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
       <c r="F6"/>
-      <c r="G6" s="100" t="s">
+      <c r="G6" s="117" t="s">
         <v>86</v>
       </c>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="117"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
@@ -2937,16 +2977,16 @@
       <c r="R6"/>
     </row>
     <row r="7" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="99"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="60">
+      <c r="B7" s="116"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="46">
         <v>1</v>
       </c>
-      <c r="E7" s="61"/>
+      <c r="E7" s="47"/>
       <c r="F7"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -2958,16 +2998,16 @@
       <c r="R7"/>
     </row>
     <row r="8" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="99"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="60">
-        <v>2</v>
+      <c r="B8" s="116"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="46">
+        <v>1.5</v>
       </c>
       <c r="F8"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="64"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="50"/>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
@@ -2979,18 +3019,18 @@
       <c r="R8"/>
     </row>
     <row r="9" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="60">
+      <c r="C9" s="46">
         <v>1</v>
       </c>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
       <c r="F9"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="65"/>
-      <c r="I9" s="64"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="50"/>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
@@ -3002,16 +3042,16 @@
       <c r="R9"/>
     </row>
     <row r="10" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="60">
+      <c r="B10" s="90"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="46">
         <v>2</v>
       </c>
-      <c r="E10" s="61"/>
+      <c r="E10" s="47"/>
       <c r="F10"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="64"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10"/>
@@ -3023,16 +3063,16 @@
       <c r="R10"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="60">
+      <c r="B11" s="90"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="46">
         <v>3</v>
       </c>
       <c r="F11"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="64"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="50"/>
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11"/>
@@ -3049,9 +3089,9 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="64"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="50"/>
       <c r="J12"/>
       <c r="K12"/>
       <c r="L12"/>
@@ -3068,9 +3108,9 @@
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="64"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="50"/>
       <c r="J13"/>
       <c r="K13"/>
       <c r="L13"/>
@@ -3087,9 +3127,9 @@
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="65"/>
-      <c r="I14" s="66"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="52"/>
       <c r="J14"/>
       <c r="K14"/>
       <c r="L14"/>
@@ -3101,21 +3141,21 @@
       <c r="R14"/>
     </row>
     <row r="15" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="102" t="s">
+      <c r="B15" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="103" t="s">
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="113" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="103"/>
-      <c r="G15" s="103"/>
-      <c r="H15" s="103" t="s">
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113" t="s">
         <v>89</v>
       </c>
-      <c r="I15" s="103"/>
-      <c r="J15" s="103"/>
+      <c r="I15" s="113"/>
+      <c r="J15" s="113"/>
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15"/>
@@ -3126,25 +3166,25 @@
       <c r="R15"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="102"/>
-      <c r="C16" s="102"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="67" t="s">
+      <c r="B16" s="112"/>
+      <c r="C16" s="112"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="67" t="s">
+      <c r="F16" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="67" t="s">
+      <c r="G16" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="67" t="s">
+      <c r="H16" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="I16" s="67" t="s">
+      <c r="I16" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="J16" s="67" t="s">
+      <c r="J16" s="53" t="s">
         <v>92</v>
       </c>
       <c r="K16"/>
@@ -3157,243 +3197,233 @@
       <c r="R16"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="104" t="s">
+      <c r="B17" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="104"/>
-      <c r="D17" s="104"/>
-      <c r="E17" s="105">
+      <c r="C17" s="106"/>
+      <c r="D17" s="106"/>
+      <c r="E17" s="108">
         <v>0.16</v>
       </c>
-      <c r="F17" s="105">
+      <c r="F17" s="108">
         <v>0.16</v>
       </c>
-      <c r="G17" s="105">
+      <c r="G17" s="108">
         <v>0.16</v>
       </c>
-      <c r="H17" s="105">
+      <c r="H17" s="108">
         <v>0.16</v>
       </c>
-      <c r="I17" s="105">
+      <c r="I17" s="108">
         <v>0.16</v>
       </c>
-      <c r="J17" s="105">
+      <c r="J17" s="108">
         <v>0.16</v>
       </c>
-      <c r="K17" s="66"/>
-      <c r="L17" s="66"/>
-      <c r="M17" s="66"/>
-      <c r="N17" s="66"/>
-      <c r="O17" s="66"/>
-      <c r="P17" s="66"/>
-      <c r="Q17" s="66"/>
-      <c r="R17" s="66"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="52"/>
+      <c r="R17" s="52"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="104" t="s">
+      <c r="B18" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="105"/>
-      <c r="I18" s="105"/>
-      <c r="J18" s="105"/>
-      <c r="K18" s="66"/>
-      <c r="L18" s="66"/>
-      <c r="M18" s="66"/>
-      <c r="N18" s="66"/>
-      <c r="O18" s="66"/>
-      <c r="P18" s="66"/>
-      <c r="Q18" s="66"/>
-      <c r="R18" s="66"/>
+      <c r="C18" s="106"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="108"/>
+      <c r="F18" s="108"/>
+      <c r="G18" s="108"/>
+      <c r="H18" s="108"/>
+      <c r="I18" s="108"/>
+      <c r="J18" s="108"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="52"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="52"/>
     </row>
     <row r="19" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="104" t="s">
+      <c r="B19" s="106" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="104"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="105">
+      <c r="C19" s="106"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="108">
         <v>0.25</v>
       </c>
-      <c r="F19" s="105">
+      <c r="F19" s="108">
         <v>0.25</v>
       </c>
-      <c r="G19" s="105">
+      <c r="G19" s="108">
         <v>0.25</v>
       </c>
-      <c r="H19" s="105">
+      <c r="H19" s="108">
         <v>0.25</v>
       </c>
-      <c r="I19" s="105">
+      <c r="I19" s="108">
         <v>0.25</v>
       </c>
-      <c r="J19" s="105">
+      <c r="J19" s="108">
         <v>0.25</v>
       </c>
-      <c r="K19" s="106"/>
-      <c r="L19" s="106"/>
-      <c r="M19" s="106"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
-      <c r="P19" s="69"/>
-      <c r="Q19" s="107"/>
-      <c r="R19" s="66"/>
+      <c r="K19" s="109"/>
+      <c r="L19" s="109"/>
+      <c r="M19" s="109"/>
+      <c r="N19" s="55"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="110"/>
+      <c r="R19" s="52"/>
     </row>
     <row r="20" spans="2:18" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="104" t="s">
+      <c r="B20" s="106" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
-      <c r="E20" s="105"/>
-      <c r="F20" s="105"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="105"/>
-      <c r="I20" s="105"/>
-      <c r="J20" s="105"/>
-      <c r="K20" s="106"/>
-      <c r="L20" s="106"/>
-      <c r="M20" s="106"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="69"/>
-      <c r="Q20" s="107"/>
-      <c r="R20" s="66"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
+      <c r="E20" s="108"/>
+      <c r="F20" s="108"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="108"/>
+      <c r="I20" s="108"/>
+      <c r="J20" s="108"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="109"/>
+      <c r="M20" s="109"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="55"/>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="110"/>
+      <c r="R20" s="52"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="104" t="s">
+      <c r="B21" s="106" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="68">
+      <c r="C21" s="106"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="54">
         <v>0.16</v>
       </c>
-      <c r="F21" s="68">
+      <c r="F21" s="54">
         <v>0.16</v>
       </c>
-      <c r="G21" s="68">
+      <c r="G21" s="54">
         <v>0.16</v>
       </c>
-      <c r="H21" s="68">
+      <c r="H21" s="54">
         <v>0.16</v>
       </c>
-      <c r="I21" s="68">
+      <c r="I21" s="54">
         <v>0.16</v>
       </c>
-      <c r="J21" s="68">
+      <c r="J21" s="54">
         <v>0.16</v>
       </c>
-      <c r="K21" s="108"/>
-      <c r="L21" s="108"/>
-      <c r="M21" s="108"/>
-      <c r="N21" s="70"/>
-      <c r="O21" s="70"/>
-      <c r="P21" s="70"/>
-      <c r="Q21" s="109"/>
-      <c r="R21" s="71"/>
+      <c r="K21" s="105"/>
+      <c r="L21" s="105"/>
+      <c r="M21" s="105"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="56"/>
+      <c r="Q21" s="107"/>
+      <c r="R21" s="57"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="104" t="s">
+      <c r="B22" s="106" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="104"/>
-      <c r="D22" s="104"/>
-      <c r="E22" s="72">
+      <c r="C22" s="106"/>
+      <c r="D22" s="106"/>
+      <c r="E22" s="58">
         <f>Servicios!C9</f>
         <v>1</v>
       </c>
-      <c r="F22" s="72">
+      <c r="F22" s="58">
         <f>Servicios!D10</f>
         <v>2</v>
       </c>
-      <c r="G22" s="72">
+      <c r="G22" s="58">
         <f>Servicios!E11</f>
         <v>3</v>
       </c>
-      <c r="H22" s="73">
+      <c r="H22" s="59">
         <f>Servicios!C6</f>
         <v>0.5</v>
       </c>
-      <c r="I22" s="74">
+      <c r="I22" s="60">
         <f>Servicios!D7</f>
         <v>1</v>
       </c>
-      <c r="J22" s="74">
+      <c r="J22" s="60">
         <f>Servicios!E8</f>
-        <v>2</v>
-      </c>
-      <c r="K22" s="108"/>
-      <c r="L22" s="108"/>
-      <c r="M22" s="108"/>
-      <c r="N22" s="70"/>
-      <c r="O22" s="70"/>
-      <c r="P22" s="70"/>
-      <c r="Q22" s="109"/>
-      <c r="R22" s="71"/>
+        <v>1.5</v>
+      </c>
+      <c r="K22" s="105"/>
+      <c r="L22" s="105"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="107"/>
+      <c r="R22" s="57"/>
     </row>
     <row r="23" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="110" t="s">
+      <c r="B23" s="104" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="110"/>
-      <c r="D23" s="110"/>
-      <c r="E23" s="75">
+      <c r="C23" s="104"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="61">
         <f t="shared" ref="E23:J23" si="0">SUM(E17:E22)</f>
         <v>1.57</v>
       </c>
-      <c r="F23" s="75">
+      <c r="F23" s="61">
         <f t="shared" si="0"/>
         <v>2.5700000000000003</v>
       </c>
-      <c r="G23" s="75">
+      <c r="G23" s="61">
         <f t="shared" si="0"/>
         <v>3.5700000000000003</v>
       </c>
-      <c r="H23" s="75">
+      <c r="H23" s="61">
         <f t="shared" si="0"/>
         <v>1.07</v>
       </c>
-      <c r="I23" s="75">
+      <c r="I23" s="61">
         <f t="shared" si="0"/>
         <v>1.57</v>
       </c>
-      <c r="J23" s="75">
+      <c r="J23" s="61">
         <f t="shared" si="0"/>
-        <v>2.5700000000000003</v>
-      </c>
-      <c r="K23" s="108"/>
-      <c r="L23" s="108"/>
-      <c r="M23" s="108"/>
-      <c r="N23" s="70"/>
-      <c r="O23" s="70"/>
-      <c r="P23" s="70"/>
-      <c r="Q23" s="64"/>
-      <c r="R23" s="71"/>
+        <v>2.0700000000000003</v>
+      </c>
+      <c r="K23" s="105"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="105"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:M20"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="G12:G14"/>
     <mergeCell ref="B15:D16"/>
     <mergeCell ref="E15:G15"/>
@@ -3406,13 +3436,23 @@
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="J17:J18"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:M20"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="K22:M22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3425,8 +3465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:X12"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X3" sqref="T3:X3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3441,7 +3481,9 @@
     <col min="8" max="8" width="12.28515625"/>
     <col min="9" max="9" width="9.7109375"/>
     <col min="10" max="10" width="11.42578125"/>
-    <col min="11" max="13" width="5"/>
+    <col min="11" max="11" width="5"/>
+    <col min="12" max="12" width="5.85546875" customWidth="1"/>
+    <col min="13" max="13" width="5"/>
     <col min="14" max="14" width="10.5703125"/>
     <col min="15" max="15" width="5"/>
     <col min="16" max="19" width="10.5703125"/>
@@ -3454,259 +3496,259 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="76"/>
-      <c r="B2" s="111" t="s">
+      <c r="A2" s="62"/>
+      <c r="B2" s="119" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111" t="s">
+      <c r="C2" s="119"/>
+      <c r="D2" s="119" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111" t="s">
+      <c r="E2" s="119"/>
+      <c r="F2" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="G2" s="111"/>
-      <c r="H2" s="77" t="s">
+      <c r="G2" s="119"/>
+      <c r="H2" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="I2" s="77" t="s">
+      <c r="I2" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="J2" s="77" t="s">
+      <c r="J2" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="K2" s="100" t="s">
+      <c r="K2" s="117" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="100"/>
-      <c r="M2" s="100"/>
-      <c r="N2" s="100"/>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="77" t="s">
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="117"/>
+      <c r="O2" s="117"/>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="R2" s="77" t="s">
+      <c r="R2" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="W2" s="116" t="s">
+      <c r="W2" s="120" t="s">
         <v>107</v>
       </c>
-      <c r="X2" s="116"/>
+      <c r="X2" s="120"/>
     </row>
     <row r="3" spans="1:24" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
-      <c r="B3" s="78" t="s">
+      <c r="A3" s="62"/>
+      <c r="B3" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="78" t="s">
+      <c r="E3" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="78" t="s">
+      <c r="F3" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="78" t="s">
+      <c r="G3" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="112" t="s">
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="L3" s="112"/>
-      <c r="M3" s="112" t="s">
+      <c r="L3" s="118"/>
+      <c r="M3" s="118" t="s">
         <v>110</v>
       </c>
-      <c r="N3" s="112"/>
-      <c r="O3" s="112" t="s">
+      <c r="N3" s="118"/>
+      <c r="O3" s="118" t="s">
         <v>92</v>
       </c>
-      <c r="P3" s="112"/>
-      <c r="Q3" s="78"/>
-      <c r="R3" s="78"/>
-      <c r="T3" s="117" t="s">
+      <c r="P3" s="118"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="T3" s="78" t="s">
         <v>111</v>
       </c>
-      <c r="U3" s="118" t="s">
+      <c r="U3" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="V3" s="119" t="s">
+      <c r="V3" s="80" t="s">
         <v>113</v>
       </c>
-      <c r="W3" s="119" t="s">
+      <c r="W3" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="X3" s="120" t="s">
+      <c r="X3" s="81" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="65" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="78">
+      <c r="B4" s="64">
         <v>6</v>
       </c>
-      <c r="C4" s="78">
+      <c r="C4" s="64">
         <v>0.5</v>
       </c>
-      <c r="D4" s="78">
+      <c r="D4" s="64">
         <v>1</v>
       </c>
-      <c r="E4" s="78">
+      <c r="E4" s="64">
         <v>1</v>
       </c>
-      <c r="F4" s="78">
+      <c r="F4" s="64">
         <v>1</v>
       </c>
-      <c r="G4" s="78">
+      <c r="G4" s="64">
         <v>1.5</v>
       </c>
-      <c r="H4" s="78">
+      <c r="H4" s="64">
         <v>8</v>
       </c>
-      <c r="I4" s="78">
+      <c r="I4" s="64">
         <f>H4*20</f>
         <v>160</v>
       </c>
-      <c r="J4" s="78">
+      <c r="J4" s="64">
         <f>I4*12</f>
         <v>1920</v>
       </c>
-      <c r="K4" s="78">
+      <c r="K4" s="64">
         <f>SUM(Servicios!H17:H21)</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="L4" s="78">
+      <c r="L4" s="64">
         <f>(K4*B4)*20</f>
         <v>68.400000000000006</v>
       </c>
-      <c r="M4" s="78">
+      <c r="M4" s="64">
         <f>SUM(Servicios!I17:I21)</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="N4" s="78">
+      <c r="N4" s="64">
         <f>(M4*D4)*20</f>
         <v>11.400000000000002</v>
       </c>
-      <c r="O4" s="78">
+      <c r="O4" s="64">
         <f>SUM(Servicios!J17:J21)</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="P4" s="78">
+      <c r="P4" s="64">
         <f>(O4*F4)*20</f>
         <v>11.400000000000002</v>
       </c>
-      <c r="Q4" s="78">
+      <c r="Q4" s="64">
         <f>SUM(L4,N4,P4)</f>
         <v>91.200000000000017</v>
       </c>
-      <c r="R4" s="78">
+      <c r="R4" s="64">
         <f>Q4*12</f>
         <v>1094.4000000000001</v>
       </c>
-      <c r="T4" s="114" t="s">
+      <c r="T4" s="76" t="s">
         <v>116</v>
       </c>
-      <c r="U4" s="78" t="s">
+      <c r="U4" s="64" t="s">
         <v>117</v>
       </c>
-      <c r="V4" s="78" t="s">
+      <c r="V4" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="W4" s="115">
+      <c r="W4" s="77">
         <v>40</v>
       </c>
-      <c r="X4" s="115">
+      <c r="X4" s="77">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="78">
+      <c r="B5" s="64">
         <v>2</v>
       </c>
-      <c r="C5" s="78">
+      <c r="C5" s="64">
         <v>1</v>
       </c>
-      <c r="D5" s="78">
+      <c r="D5" s="64">
         <v>1</v>
       </c>
-      <c r="E5" s="78">
+      <c r="E5" s="64">
         <v>2</v>
       </c>
-      <c r="F5" s="78">
+      <c r="F5" s="64">
         <v>1</v>
       </c>
-      <c r="G5" s="78">
+      <c r="G5" s="64">
         <v>3</v>
       </c>
-      <c r="H5" s="78">
+      <c r="H5" s="64">
         <v>3</v>
       </c>
-      <c r="I5" s="78">
+      <c r="I5" s="64">
         <f>H5*20</f>
         <v>60</v>
       </c>
-      <c r="J5" s="78">
+      <c r="J5" s="64">
         <f>I5*12</f>
         <v>720</v>
       </c>
-      <c r="K5" s="78">
+      <c r="K5" s="64">
         <f>SUM(Servicios!E17:E21)</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="L5" s="78">
+      <c r="L5" s="64">
         <f>(K5*B5)*20</f>
         <v>22.800000000000004</v>
       </c>
-      <c r="M5" s="78">
+      <c r="M5" s="64">
         <f>SUM(Servicios!F17:F21)</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="N5" s="78">
+      <c r="N5" s="64">
         <f>(M5*D5)*20</f>
         <v>11.400000000000002</v>
       </c>
-      <c r="O5" s="78">
+      <c r="O5" s="64">
         <f>SUM(Servicios!G17:G21)</f>
         <v>0.57000000000000006</v>
       </c>
-      <c r="P5" s="78">
+      <c r="P5" s="64">
         <f>(O5*F5)*20</f>
         <v>11.400000000000002</v>
       </c>
-      <c r="Q5" s="78">
+      <c r="Q5" s="64">
         <f>SUM(L5,N5,P5)</f>
         <v>45.600000000000009</v>
       </c>
-      <c r="R5" s="78">
+      <c r="R5" s="64">
         <f>Q5*12</f>
         <v>547.20000000000005</v>
       </c>
-      <c r="T5" s="114" t="s">
+      <c r="T5" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="U5" s="78" t="s">
+      <c r="U5" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="V5" s="113" t="s">
+      <c r="V5" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="W5" s="113" t="s">
+      <c r="W5" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="X5" s="113" t="s">
+      <c r="X5" s="75" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3716,56 +3758,57 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="80"/>
-      <c r="B9" s="77" t="s">
+      <c r="A9" s="66"/>
+      <c r="B9" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="77" t="s">
+      <c r="C9" s="66"/>
+      <c r="D9" s="63" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="67" t="s">
         <v>127</v>
       </c>
-      <c r="B10" s="78">
+      <c r="B10" s="64">
         <v>1</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78">
+      <c r="C10" s="64"/>
+      <c r="D10" s="64">
         <f>B10*12</f>
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="78">
+      <c r="B11" s="64">
         <v>2</v>
       </c>
-      <c r="C11" s="78"/>
-      <c r="D11" s="78">
+      <c r="C11" s="64"/>
+      <c r="D11" s="64">
         <f>B11*12</f>
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="79" t="s">
+      <c r="A12" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="78">
+      <c r="B12" s="64">
         <v>0.5</v>
       </c>
-      <c r="C12" s="78"/>
-      <c r="D12" s="82">
+      <c r="C12" s="64"/>
+      <c r="D12" s="68">
         <f>B12*12</f>
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="W2:X2"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="O3:P3"/>
@@ -3773,7 +3816,6 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="K2:P2"/>
-    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3786,9 +3828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3801,85 +3841,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="69" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="70" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="86" t="s">
+      <c r="A3" s="72" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="73" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="72" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="74" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="72" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="83" t="s">
+      <c r="A7" s="69" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="84" t="s">
+      <c r="A8" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="70" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="72" t="s">
         <v>136</v>
       </c>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="72" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="86" t="s">
+      <c r="A10" s="72" t="s">
         <v>139</v>
       </c>
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="72" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="86" t="s">
+      <c r="C10" s="72" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="72" t="s">
         <v>142</v>
       </c>
     </row>

</xml_diff>